<commit_message>
updated poisson sql model
</commit_message>
<xml_diff>
--- a/picks.xlsx
+++ b/picks.xlsx
@@ -1,31 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leonard\gitboyzorro5\FDAS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Magut\FDAS\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C4C4288-374F-4DF6-873D-DEBA63D77A01}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7350"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2409-2809" sheetId="1" r:id="rId1"/>
     <sheet name="2909-1005" sheetId="2" r:id="rId2"/>
+    <sheet name="1008-1010" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1996" uniqueCount="410">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2230" uniqueCount="410">
   <si>
     <t>Div</t>
   </si>
@@ -1260,7 +1268,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1589,10 +1597,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R182"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A151" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A160" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="A157" sqref="A157:XFD157"/>
     </sheetView>
   </sheetViews>
@@ -10705,11 +10713,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:T192"/>
   <sheetViews>
     <sheetView zoomScale="81" zoomScaleNormal="81" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20319,4 +20327,2370 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F88832EC-F636-43FB-BE3C-0BC0F9DD8ED0}">
+  <dimension ref="A1:T47"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="V19" sqref="V19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="17.140625" customWidth="1"/>
+    <col min="3" max="4" width="16.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2">
+        <v>1</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="2">
+        <v>2</v>
+      </c>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="L1" s="1"/>
+      <c r="N1" s="2">
+        <v>1</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="P1" s="2">
+        <v>2</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="T1" s="1"/>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B2" t="s">
+        <v>136</v>
+      </c>
+      <c r="C2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D2" s="4">
+        <v>44478</v>
+      </c>
+      <c r="F2" s="5">
+        <v>0.54951335847795557</v>
+      </c>
+      <c r="G2" s="5">
+        <v>0.21327568406915384</v>
+      </c>
+      <c r="H2" s="5">
+        <v>0.22344462311207067</v>
+      </c>
+      <c r="J2" s="5">
+        <v>0.66329363965260968</v>
+      </c>
+      <c r="K2" s="5">
+        <v>0.33007815722445061</v>
+      </c>
+      <c r="L2" t="s">
+        <v>16</v>
+      </c>
+      <c r="N2" s="5">
+        <v>0.6415274880203885</v>
+      </c>
+      <c r="O2" s="5">
+        <v>0.19954611926188734</v>
+      </c>
+      <c r="P2" s="5">
+        <v>0.15115893141584474</v>
+      </c>
+      <c r="R2" s="5">
+        <v>0.61030732991638148</v>
+      </c>
+      <c r="S2" s="5">
+        <v>0.38214231770395135</v>
+      </c>
+      <c r="T2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D3" s="4">
+        <v>44478</v>
+      </c>
+      <c r="F3" s="5">
+        <v>0.30689064301484109</v>
+      </c>
+      <c r="G3" s="5">
+        <v>0.29941675298476805</v>
+      </c>
+      <c r="H3" s="5">
+        <v>0.36393794973474275</v>
+      </c>
+      <c r="J3" s="5">
+        <v>0.34648834032400666</v>
+      </c>
+      <c r="K3" s="5">
+        <v>0.65327444916694111</v>
+      </c>
+      <c r="L3" t="s">
+        <v>20</v>
+      </c>
+      <c r="N3" s="5">
+        <v>0.35946460128159646</v>
+      </c>
+      <c r="O3" s="5">
+        <v>0.29476290548159712</v>
+      </c>
+      <c r="P3" s="5">
+        <v>0.32247697211538234</v>
+      </c>
+      <c r="R3" s="5">
+        <v>0.36637333766116359</v>
+      </c>
+      <c r="S3" s="5">
+        <v>0.63335946191532611</v>
+      </c>
+      <c r="T3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B4" t="s">
+        <v>123</v>
+      </c>
+      <c r="C4" t="s">
+        <v>129</v>
+      </c>
+      <c r="D4" s="4">
+        <v>44478</v>
+      </c>
+      <c r="F4" s="5">
+        <v>0.30819630401610187</v>
+      </c>
+      <c r="G4" s="5">
+        <v>0.23891674710065408</v>
+      </c>
+      <c r="H4" s="5">
+        <v>0.41307803075356853</v>
+      </c>
+      <c r="J4" s="5">
+        <v>0.58047782084569199</v>
+      </c>
+      <c r="K4" s="5">
+        <v>0.41727608919300396</v>
+      </c>
+      <c r="L4" t="s">
+        <v>28</v>
+      </c>
+      <c r="N4" s="5">
+        <v>0.63397024359804754</v>
+      </c>
+      <c r="O4" s="5">
+        <v>0.31271071166098491</v>
+      </c>
+      <c r="P4" s="5">
+        <v>5.3037846414225126E-2</v>
+      </c>
+      <c r="R4" s="5">
+        <v>0.15607463081161191</v>
+      </c>
+      <c r="S4" s="5">
+        <v>0.84369200306599523</v>
+      </c>
+      <c r="T4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>112</v>
+      </c>
+      <c r="B5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C5" t="s">
+        <v>125</v>
+      </c>
+      <c r="D5" s="4">
+        <v>44478</v>
+      </c>
+      <c r="F5" s="5">
+        <v>0.29513730940331806</v>
+      </c>
+      <c r="G5" s="5">
+        <v>0.19992223424637309</v>
+      </c>
+      <c r="H5" s="5">
+        <v>0.45964953833647815</v>
+      </c>
+      <c r="J5" s="5">
+        <v>0.76117400256539269</v>
+      </c>
+      <c r="K5" s="5">
+        <v>0.22692723666145001</v>
+      </c>
+      <c r="L5" t="s">
+        <v>11</v>
+      </c>
+      <c r="N5" s="5">
+        <v>0.48796743653448743</v>
+      </c>
+      <c r="O5" s="5">
+        <v>0.23227300090214831</v>
+      </c>
+      <c r="P5" s="5">
+        <v>0.26274904212244299</v>
+      </c>
+      <c r="R5" s="5">
+        <v>0.60380104598457751</v>
+      </c>
+      <c r="S5" s="5">
+        <v>0.39306129316240118</v>
+      </c>
+      <c r="T5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>112</v>
+      </c>
+      <c r="B6" t="s">
+        <v>132</v>
+      </c>
+      <c r="C6" t="s">
+        <v>120</v>
+      </c>
+      <c r="D6" s="4">
+        <v>44478</v>
+      </c>
+      <c r="F6" s="5">
+        <v>0.27838171973625336</v>
+      </c>
+      <c r="G6" s="5">
+        <v>0.32933554379035801</v>
+      </c>
+      <c r="H6" s="5">
+        <v>0.36475271756906796</v>
+      </c>
+      <c r="J6" s="5">
+        <v>0.26202740609296599</v>
+      </c>
+      <c r="K6" s="5">
+        <v>0.7378761593305545</v>
+      </c>
+      <c r="L6" t="s">
+        <v>20</v>
+      </c>
+      <c r="N6" s="5">
+        <v>0.82219700101710813</v>
+      </c>
+      <c r="O6" s="5">
+        <v>0.12072152171681116</v>
+      </c>
+      <c r="P6" s="5">
+        <v>4.2811348657909573E-2</v>
+      </c>
+      <c r="R6" s="5">
+        <v>0.63037550520608954</v>
+      </c>
+      <c r="S6" s="5">
+        <v>0.3426471381643364</v>
+      </c>
+      <c r="T6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>112</v>
+      </c>
+      <c r="B7" t="s">
+        <v>122</v>
+      </c>
+      <c r="C7" t="s">
+        <v>124</v>
+      </c>
+      <c r="D7" s="4">
+        <v>44478</v>
+      </c>
+      <c r="F7" s="5">
+        <v>0.43795715365942123</v>
+      </c>
+      <c r="G7" s="5">
+        <v>0.24844394052349156</v>
+      </c>
+      <c r="H7" s="5">
+        <v>0.29303564501154727</v>
+      </c>
+      <c r="J7" s="5">
+        <v>0.54364946290729921</v>
+      </c>
+      <c r="K7" s="5">
+        <v>0.45475868345202108</v>
+      </c>
+      <c r="L7" t="s">
+        <v>16</v>
+      </c>
+      <c r="N7" s="5">
+        <v>0.77351223766594335</v>
+      </c>
+      <c r="O7" s="5">
+        <v>0.17652052596667381</v>
+      </c>
+      <c r="P7" s="5">
+        <v>4.7814106960658666E-2</v>
+      </c>
+      <c r="R7" s="5">
+        <v>0.39510874069716606</v>
+      </c>
+      <c r="S7" s="5">
+        <v>0.60064365592633961</v>
+      </c>
+      <c r="T7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>112</v>
+      </c>
+      <c r="B8" t="s">
+        <v>114</v>
+      </c>
+      <c r="C8" t="s">
+        <v>126</v>
+      </c>
+      <c r="D8" s="4">
+        <v>44478</v>
+      </c>
+      <c r="F8" s="5">
+        <v>0.36166788695290819</v>
+      </c>
+      <c r="G8" s="5">
+        <v>0.2625855669234986</v>
+      </c>
+      <c r="H8" s="5">
+        <v>0.34724977232577547</v>
+      </c>
+      <c r="J8" s="5">
+        <v>0.48896072817252867</v>
+      </c>
+      <c r="K8" s="5">
+        <v>0.51016858542707966</v>
+      </c>
+      <c r="L8" t="s">
+        <v>20</v>
+      </c>
+      <c r="N8" s="5">
+        <v>0.43043474799092779</v>
+      </c>
+      <c r="O8" s="5">
+        <v>0.23700449402428098</v>
+      </c>
+      <c r="P8" s="5">
+        <v>0.30978856918388903</v>
+      </c>
+      <c r="R8" s="5">
+        <v>0.60549168799950459</v>
+      </c>
+      <c r="S8" s="5">
+        <v>0.39193187107281907</v>
+      </c>
+      <c r="T8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>112</v>
+      </c>
+      <c r="B9" t="s">
+        <v>137</v>
+      </c>
+      <c r="C9" t="s">
+        <v>128</v>
+      </c>
+      <c r="D9" s="4">
+        <v>44478</v>
+      </c>
+      <c r="F9" s="5">
+        <v>0.17863887389371408</v>
+      </c>
+      <c r="G9" s="5">
+        <v>0.24897436892522432</v>
+      </c>
+      <c r="H9" s="5">
+        <v>0.50705983522392895</v>
+      </c>
+      <c r="J9" s="5">
+        <v>0.42207247726304153</v>
+      </c>
+      <c r="K9" s="5">
+        <v>0.57655848315481706</v>
+      </c>
+      <c r="L9" t="s">
+        <v>28</v>
+      </c>
+      <c r="N9" s="5">
+        <v>0.52547116254786685</v>
+      </c>
+      <c r="O9" s="5">
+        <v>0.26533593365711938</v>
+      </c>
+      <c r="P9" s="5">
+        <v>0.20015909888356453</v>
+      </c>
+      <c r="R9" s="5">
+        <v>0.40474349624705791</v>
+      </c>
+      <c r="S9" s="5">
+        <v>0.59437216515951208</v>
+      </c>
+      <c r="T9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>112</v>
+      </c>
+      <c r="B10" t="s">
+        <v>119</v>
+      </c>
+      <c r="C10" t="s">
+        <v>130</v>
+      </c>
+      <c r="D10" s="4">
+        <v>44478</v>
+      </c>
+      <c r="F10" s="5">
+        <v>0.11599499884270288</v>
+      </c>
+      <c r="G10" s="5">
+        <v>0.18860256046004345</v>
+      </c>
+      <c r="H10" s="5">
+        <v>0.59736108782743869</v>
+      </c>
+      <c r="J10" s="5">
+        <v>0.53595071325838972</v>
+      </c>
+      <c r="K10" s="5">
+        <v>0.45788545756356336</v>
+      </c>
+      <c r="L10" t="s">
+        <v>28</v>
+      </c>
+      <c r="N10" s="5">
+        <v>0.52728340884217761</v>
+      </c>
+      <c r="O10" s="5">
+        <v>0.28790220198582633</v>
+      </c>
+      <c r="P10" s="5">
+        <v>0.17853637244752327</v>
+      </c>
+      <c r="R10" s="5">
+        <v>0.31624821616661031</v>
+      </c>
+      <c r="S10" s="5">
+        <v>0.68330370559109477</v>
+      </c>
+      <c r="T10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>112</v>
+      </c>
+      <c r="B11" t="s">
+        <v>117</v>
+      </c>
+      <c r="C11" t="s">
+        <v>127</v>
+      </c>
+      <c r="D11" s="4">
+        <v>44478</v>
+      </c>
+      <c r="F11" s="5">
+        <v>0.41272658787247024</v>
+      </c>
+      <c r="G11" s="5">
+        <v>0.24450747459087113</v>
+      </c>
+      <c r="H11" s="5">
+        <v>0.31868552769730196</v>
+      </c>
+      <c r="J11" s="5">
+        <v>0.57069498894209758</v>
+      </c>
+      <c r="K11" s="5">
+        <v>0.42745257478237575</v>
+      </c>
+      <c r="L11" t="s">
+        <v>16</v>
+      </c>
+      <c r="N11" s="5">
+        <v>0.83058204321075013</v>
+      </c>
+      <c r="O11" s="5">
+        <v>0.12781985219639877</v>
+      </c>
+      <c r="P11" s="5">
+        <v>3.4156692957580607E-2</v>
+      </c>
+      <c r="R11" s="5">
+        <v>0.51887933090423077</v>
+      </c>
+      <c r="S11" s="5">
+        <v>0.46764102682907033</v>
+      </c>
+      <c r="T11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>112</v>
+      </c>
+      <c r="B12" t="s">
+        <v>131</v>
+      </c>
+      <c r="C12" t="s">
+        <v>121</v>
+      </c>
+      <c r="D12" s="4">
+        <v>44478</v>
+      </c>
+      <c r="F12" s="5">
+        <v>0.40601743710753585</v>
+      </c>
+      <c r="G12" s="5">
+        <v>0.26654869057487085</v>
+      </c>
+      <c r="H12" s="5">
+        <v>0.30546153637552692</v>
+      </c>
+      <c r="J12" s="5">
+        <v>0.46846102492727637</v>
+      </c>
+      <c r="K12" s="5">
+        <v>0.53077416036017044</v>
+      </c>
+      <c r="L12" t="s">
+        <v>20</v>
+      </c>
+      <c r="N12" s="5">
+        <v>7.172894132323282E-2</v>
+      </c>
+      <c r="O12" s="5">
+        <v>0.28271770471994506</v>
+      </c>
+      <c r="P12" s="5">
+        <v>0.56604441645208226</v>
+      </c>
+      <c r="R12" s="5">
+        <v>0.21135939369253112</v>
+      </c>
+      <c r="S12" s="5">
+        <v>0.78819686529908972</v>
+      </c>
+      <c r="T12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>112</v>
+      </c>
+      <c r="B13" t="s">
+        <v>134</v>
+      </c>
+      <c r="C13" t="s">
+        <v>115</v>
+      </c>
+      <c r="D13" s="4">
+        <v>44478</v>
+      </c>
+      <c r="F13" s="5">
+        <v>0.41444496126079339</v>
+      </c>
+      <c r="G13" s="5">
+        <v>0.36000675594584614</v>
+      </c>
+      <c r="H13" s="5">
+        <v>0.21804785650222053</v>
+      </c>
+      <c r="J13" s="5">
+        <v>0.19095781962606953</v>
+      </c>
+      <c r="K13" s="5">
+        <v>0.80899227981442423</v>
+      </c>
+      <c r="L13" t="s">
+        <v>20</v>
+      </c>
+      <c r="N13" s="5">
+        <v>0.768112820988476</v>
+      </c>
+      <c r="O13" s="5">
+        <v>0.16150727163853429</v>
+      </c>
+      <c r="P13" s="5">
+        <v>6.5986381327827082E-2</v>
+      </c>
+      <c r="R13" s="5">
+        <v>0.52591915587291849</v>
+      </c>
+      <c r="S13" s="5">
+        <v>0.46470281311718464</v>
+      </c>
+      <c r="T13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>138</v>
+      </c>
+      <c r="B14" t="s">
+        <v>152</v>
+      </c>
+      <c r="C14" t="s">
+        <v>140</v>
+      </c>
+      <c r="D14" s="4">
+        <v>44478</v>
+      </c>
+      <c r="F14" s="5">
+        <v>0.51475799948675804</v>
+      </c>
+      <c r="G14" s="5">
+        <v>0.27877513115591634</v>
+      </c>
+      <c r="H14" s="5">
+        <v>0.19809904420378405</v>
+      </c>
+      <c r="J14" s="5">
+        <v>0.35953527049498618</v>
+      </c>
+      <c r="K14" s="5">
+        <v>0.639886279127163</v>
+      </c>
+      <c r="L14" t="s">
+        <v>20</v>
+      </c>
+      <c r="N14" s="5">
+        <v>0.6876140884540699</v>
+      </c>
+      <c r="O14" s="5">
+        <v>0.20228891538524565</v>
+      </c>
+      <c r="P14" s="5">
+        <v>0.10653988754644303</v>
+      </c>
+      <c r="R14" s="5">
+        <v>0.4819014969156864</v>
+      </c>
+      <c r="S14" s="5">
+        <v>0.51377737237712806</v>
+      </c>
+      <c r="T14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>138</v>
+      </c>
+      <c r="B15" t="s">
+        <v>142</v>
+      </c>
+      <c r="C15" t="s">
+        <v>144</v>
+      </c>
+      <c r="D15" s="4">
+        <v>44478</v>
+      </c>
+      <c r="F15" s="5">
+        <v>0.28598954991406095</v>
+      </c>
+      <c r="G15" s="5">
+        <v>0.31755854913172193</v>
+      </c>
+      <c r="H15" s="5">
+        <v>0.36747938614634307</v>
+      </c>
+      <c r="J15" s="5">
+        <v>0.29170865393937606</v>
+      </c>
+      <c r="K15" s="5">
+        <v>0.7081545082016717</v>
+      </c>
+      <c r="L15" t="s">
+        <v>20</v>
+      </c>
+      <c r="N15" s="5">
+        <v>0.386722551446818</v>
+      </c>
+      <c r="O15" s="5">
+        <v>0.29266883314425401</v>
+      </c>
+      <c r="P15" s="5">
+        <v>0.30045649655099743</v>
+      </c>
+      <c r="R15" s="5">
+        <v>0.37092506502823569</v>
+      </c>
+      <c r="S15" s="5">
+        <v>0.62878026286438571</v>
+      </c>
+      <c r="T15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>138</v>
+      </c>
+      <c r="B16" t="s">
+        <v>162</v>
+      </c>
+      <c r="C16" t="s">
+        <v>146</v>
+      </c>
+      <c r="D16" s="4">
+        <v>44478</v>
+      </c>
+      <c r="F16" s="5">
+        <v>0.65142331897682137</v>
+      </c>
+      <c r="G16" s="5">
+        <v>0.24504542773916863</v>
+      </c>
+      <c r="H16" s="5">
+        <v>0.10152390691388959</v>
+      </c>
+      <c r="J16" s="5">
+        <v>0.32972588303182826</v>
+      </c>
+      <c r="K16" s="5">
+        <v>0.6690546098486948</v>
+      </c>
+      <c r="L16" t="s">
+        <v>37</v>
+      </c>
+      <c r="N16" s="5">
+        <v>0.4120892704617426</v>
+      </c>
+      <c r="O16" s="5">
+        <v>0.41709126316952638</v>
+      </c>
+      <c r="P16" s="5">
+        <v>0.16779753621597435</v>
+      </c>
+      <c r="R16" s="5">
+        <v>0.10992012485699187</v>
+      </c>
+      <c r="S16" s="5">
+        <v>0.89006417107147906</v>
+      </c>
+      <c r="T16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>138</v>
+      </c>
+      <c r="B17" t="s">
+        <v>155</v>
+      </c>
+      <c r="C17" t="s">
+        <v>139</v>
+      </c>
+      <c r="D17" s="4">
+        <v>44478</v>
+      </c>
+      <c r="F17" s="5">
+        <v>0.31300600284943997</v>
+      </c>
+      <c r="G17" s="5">
+        <v>0.24323791027052896</v>
+      </c>
+      <c r="H17" s="5">
+        <v>0.40522008574112661</v>
+      </c>
+      <c r="J17" s="5">
+        <v>0.56276621999893428</v>
+      </c>
+      <c r="K17" s="5">
+        <v>0.43534591520562249</v>
+      </c>
+      <c r="L17" t="s">
+        <v>28</v>
+      </c>
+      <c r="N17" s="5">
+        <v>0.417240618899196</v>
+      </c>
+      <c r="O17" s="5">
+        <v>0.34596782597301545</v>
+      </c>
+      <c r="P17" s="5">
+        <v>0.227928989080595</v>
+      </c>
+      <c r="R17" s="5">
+        <v>0.21783664789342991</v>
+      </c>
+      <c r="S17" s="5">
+        <v>0.78209294490233561</v>
+      </c>
+      <c r="T17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>138</v>
+      </c>
+      <c r="B18" t="s">
+        <v>160</v>
+      </c>
+      <c r="C18" t="s">
+        <v>148</v>
+      </c>
+      <c r="D18" s="4">
+        <v>44478</v>
+      </c>
+      <c r="F18" s="5">
+        <v>0.3666988873478893</v>
+      </c>
+      <c r="G18" s="5">
+        <v>0.28374589420401808</v>
+      </c>
+      <c r="H18" s="5">
+        <v>0.3252528920285363</v>
+      </c>
+      <c r="J18" s="5">
+        <v>0.40462766754126339</v>
+      </c>
+      <c r="K18" s="5">
+        <v>0.59497777378629924</v>
+      </c>
+      <c r="L18" t="s">
+        <v>20</v>
+      </c>
+      <c r="N18" s="5">
+        <v>0.25366426121097624</v>
+      </c>
+      <c r="O18" s="5">
+        <v>0.30699624403576414</v>
+      </c>
+      <c r="P18" s="5">
+        <v>0.40305566359177919</v>
+      </c>
+      <c r="R18" s="5">
+        <v>0.30811312865491208</v>
+      </c>
+      <c r="S18" s="5">
+        <v>0.69167358643720778</v>
+      </c>
+      <c r="T18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>138</v>
+      </c>
+      <c r="B19" t="s">
+        <v>151</v>
+      </c>
+      <c r="C19" t="s">
+        <v>149</v>
+      </c>
+      <c r="D19" s="4">
+        <v>44478</v>
+      </c>
+      <c r="F19" s="5">
+        <v>0.43511842094129638</v>
+      </c>
+      <c r="G19" s="5">
+        <v>0.26213180083731025</v>
+      </c>
+      <c r="H19" s="5">
+        <v>0.28369219690247988</v>
+      </c>
+      <c r="J19" s="5">
+        <v>0.47925671644595386</v>
+      </c>
+      <c r="K19" s="5">
+        <v>0.51981312271421565</v>
+      </c>
+      <c r="L19" t="s">
+        <v>20</v>
+      </c>
+      <c r="N19" s="5">
+        <v>0.40065268453592651</v>
+      </c>
+      <c r="O19" s="5">
+        <v>0.20778601146853151</v>
+      </c>
+      <c r="P19" s="5">
+        <v>0.36172214518573298</v>
+      </c>
+      <c r="R19" s="5">
+        <v>0.76539230258911795</v>
+      </c>
+      <c r="S19" s="5">
+        <v>0.22434029286407406</v>
+      </c>
+      <c r="T19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>138</v>
+      </c>
+      <c r="B20" t="s">
+        <v>147</v>
+      </c>
+      <c r="C20" t="s">
+        <v>154</v>
+      </c>
+      <c r="D20" s="4">
+        <v>44478</v>
+      </c>
+      <c r="F20" s="5">
+        <v>0.67454180410226405</v>
+      </c>
+      <c r="G20" s="5">
+        <v>0.21427843607169667</v>
+      </c>
+      <c r="H20" s="5">
+        <v>0.10806756554210252</v>
+      </c>
+      <c r="J20" s="5">
+        <v>0.43842415863382828</v>
+      </c>
+      <c r="K20" s="5">
+        <v>0.55857111440587615</v>
+      </c>
+      <c r="L20" t="s">
+        <v>16</v>
+      </c>
+      <c r="N20" s="5">
+        <v>0.4093115155641564</v>
+      </c>
+      <c r="O20" s="5">
+        <v>0.46516688339351886</v>
+      </c>
+      <c r="P20" s="5">
+        <v>0.12440735431447052</v>
+      </c>
+      <c r="R20" s="5">
+        <v>6.8236153891286011E-2</v>
+      </c>
+      <c r="S20" s="5">
+        <v>0.9317568243930302</v>
+      </c>
+      <c r="T20" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>138</v>
+      </c>
+      <c r="B21" t="s">
+        <v>150</v>
+      </c>
+      <c r="C21" t="s">
+        <v>156</v>
+      </c>
+      <c r="D21" s="4">
+        <v>44478</v>
+      </c>
+      <c r="F21" s="5">
+        <v>0.34653429396474889</v>
+      </c>
+      <c r="G21" s="5">
+        <v>0.20481228519490485</v>
+      </c>
+      <c r="H21" s="5">
+        <v>0.41171901454185145</v>
+      </c>
+      <c r="J21" s="5">
+        <v>0.76726331158586725</v>
+      </c>
+      <c r="K21" s="5">
+        <v>0.22181895872908536</v>
+      </c>
+      <c r="L21" t="s">
+        <v>11</v>
+      </c>
+      <c r="N21" s="5">
+        <v>0.52458448457594142</v>
+      </c>
+      <c r="O21" s="5">
+        <v>0.24107000985980501</v>
+      </c>
+      <c r="P21" s="5">
+        <v>0.22214099038570648</v>
+      </c>
+      <c r="R21" s="5">
+        <v>0.52380394840828914</v>
+      </c>
+      <c r="S21" s="5">
+        <v>0.47409536391627954</v>
+      </c>
+      <c r="T21" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>138</v>
+      </c>
+      <c r="B22" t="s">
+        <v>143</v>
+      </c>
+      <c r="C22" t="s">
+        <v>158</v>
+      </c>
+      <c r="D22" s="4">
+        <v>44478</v>
+      </c>
+      <c r="F22" s="5">
+        <v>0.6495628424751726</v>
+      </c>
+      <c r="G22" s="5">
+        <v>0.21047006155783396</v>
+      </c>
+      <c r="H22" s="5">
+        <v>0.1347187692569739</v>
+      </c>
+      <c r="J22" s="5">
+        <v>0.51702420753353717</v>
+      </c>
+      <c r="K22" s="5">
+        <v>0.47868774982099765</v>
+      </c>
+      <c r="L22" t="s">
+        <v>16</v>
+      </c>
+      <c r="N22" s="5">
+        <v>0.39746883897707863</v>
+      </c>
+      <c r="O22" s="5">
+        <v>0.33906193084489106</v>
+      </c>
+      <c r="P22" s="5">
+        <v>0.25189696364350539</v>
+      </c>
+      <c r="R22" s="5">
+        <v>0.23817359554680434</v>
+      </c>
+      <c r="S22" s="5">
+        <v>0.76175039257260713</v>
+      </c>
+      <c r="T22" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>138</v>
+      </c>
+      <c r="B23" t="s">
+        <v>141</v>
+      </c>
+      <c r="C23" t="s">
+        <v>153</v>
+      </c>
+      <c r="D23" s="4">
+        <v>44478</v>
+      </c>
+      <c r="F23" s="5">
+        <v>0.23211462195824978</v>
+      </c>
+      <c r="G23" s="5">
+        <v>0.37674878584384913</v>
+      </c>
+      <c r="H23" s="5">
+        <v>0.36727150596636443</v>
+      </c>
+      <c r="J23" s="5">
+        <v>0.16772958318695921</v>
+      </c>
+      <c r="K23" s="5">
+        <v>0.83224080096135467</v>
+      </c>
+      <c r="L23" t="s">
+        <v>20</v>
+      </c>
+      <c r="N23" s="5">
+        <v>0.5080186347571134</v>
+      </c>
+      <c r="O23" s="5">
+        <v>0.24221810287268533</v>
+      </c>
+      <c r="P23" s="5">
+        <v>0.23605117098048486</v>
+      </c>
+      <c r="R23" s="5">
+        <v>0.53293209445108514</v>
+      </c>
+      <c r="S23" s="5">
+        <v>0.46502574794733098</v>
+      </c>
+      <c r="T23" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>138</v>
+      </c>
+      <c r="B24" t="s">
+        <v>159</v>
+      </c>
+      <c r="C24" t="s">
+        <v>157</v>
+      </c>
+      <c r="D24" s="4">
+        <v>44478</v>
+      </c>
+      <c r="F24" s="5">
+        <v>0.44484302055892549</v>
+      </c>
+      <c r="G24" s="5">
+        <v>0.28298301332659398</v>
+      </c>
+      <c r="H24" s="5">
+        <v>0.25733404805069759</v>
+      </c>
+      <c r="J24" s="5">
+        <v>0.38824298673292246</v>
+      </c>
+      <c r="K24" s="5">
+        <v>0.61130229066439346</v>
+      </c>
+      <c r="L24" t="s">
+        <v>20</v>
+      </c>
+      <c r="N24" s="5">
+        <v>0.71936223708925429</v>
+      </c>
+      <c r="O24" s="5">
+        <v>0.1887017064334901</v>
+      </c>
+      <c r="P24" s="5">
+        <v>8.8713418723274803E-2</v>
+      </c>
+      <c r="R24" s="5">
+        <v>0.48711124215801033</v>
+      </c>
+      <c r="S24" s="5">
+        <v>0.50745473378375527</v>
+      </c>
+      <c r="T24" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>138</v>
+      </c>
+      <c r="B25" t="s">
+        <v>161</v>
+      </c>
+      <c r="C25" t="s">
+        <v>145</v>
+      </c>
+      <c r="D25" s="4">
+        <v>44478</v>
+      </c>
+      <c r="F25" s="5">
+        <v>0.59583425838326509</v>
+      </c>
+      <c r="G25" s="5">
+        <v>0.20499690669050349</v>
+      </c>
+      <c r="H25" s="5">
+        <v>0.1881425892721674</v>
+      </c>
+      <c r="J25" s="5">
+        <v>0.65600216691171731</v>
+      </c>
+      <c r="K25" s="5">
+        <v>0.33597706449925452</v>
+      </c>
+      <c r="L25" t="s">
+        <v>16</v>
+      </c>
+      <c r="N25" s="5">
+        <v>0.25322471749430786</v>
+      </c>
+      <c r="O25" s="5">
+        <v>0.23717644617880751</v>
+      </c>
+      <c r="P25" s="5">
+        <v>0.45919837041825196</v>
+      </c>
+      <c r="R25" s="5">
+        <v>0.54919840333503922</v>
+      </c>
+      <c r="S25" s="5">
+        <v>0.44850483083491133</v>
+      </c>
+      <c r="T25" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>163</v>
+      </c>
+      <c r="B26" t="s">
+        <v>166</v>
+      </c>
+      <c r="C26" t="s">
+        <v>185</v>
+      </c>
+      <c r="D26" s="4">
+        <v>44478</v>
+      </c>
+      <c r="F26" s="5">
+        <v>0.24372206571355148</v>
+      </c>
+      <c r="G26" s="5">
+        <v>0.24487646969724483</v>
+      </c>
+      <c r="H26" s="5">
+        <v>0.46007662087277218</v>
+      </c>
+      <c r="J26" s="5">
+        <v>0.50790031714221051</v>
+      </c>
+      <c r="K26" s="5">
+        <v>0.49038234597995395</v>
+      </c>
+      <c r="L26" t="s">
+        <v>28</v>
+      </c>
+      <c r="N26" s="5">
+        <v>0.66390882170597498</v>
+      </c>
+      <c r="O26" s="5">
+        <v>0.21088950374605336</v>
+      </c>
+      <c r="P26" s="5">
+        <v>0.12105820300603866</v>
+      </c>
+      <c r="R26" s="5">
+        <v>0.48285280736167452</v>
+      </c>
+      <c r="S26" s="5">
+        <v>0.51339349395787304</v>
+      </c>
+      <c r="T26" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>163</v>
+      </c>
+      <c r="B27" t="s">
+        <v>171</v>
+      </c>
+      <c r="C27" t="s">
+        <v>176</v>
+      </c>
+      <c r="D27" s="4">
+        <v>44478</v>
+      </c>
+      <c r="F27" s="5">
+        <v>0.31987516640089991</v>
+      </c>
+      <c r="G27" s="5">
+        <v>0.2916583844898219</v>
+      </c>
+      <c r="H27" s="5">
+        <v>0.359053495141891</v>
+      </c>
+      <c r="J27" s="5">
+        <v>0.37351623496086794</v>
+      </c>
+      <c r="K27" s="5">
+        <v>0.62617998797035834</v>
+      </c>
+      <c r="L27" t="s">
+        <v>20</v>
+      </c>
+      <c r="N27" s="5">
+        <v>0.3452554725267602</v>
+      </c>
+      <c r="O27" s="5">
+        <v>0.4149783441069726</v>
+      </c>
+      <c r="P27" s="5">
+        <v>0.2327087977790184</v>
+      </c>
+      <c r="R27" s="5">
+        <v>0.12302366225634015</v>
+      </c>
+      <c r="S27" s="5">
+        <v>0.87696695678830061</v>
+      </c>
+      <c r="T27" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>163</v>
+      </c>
+      <c r="B28" t="s">
+        <v>180</v>
+      </c>
+      <c r="C28" t="s">
+        <v>174</v>
+      </c>
+      <c r="D28" s="4">
+        <v>44478</v>
+      </c>
+      <c r="F28" s="5">
+        <v>0.20914908969785362</v>
+      </c>
+      <c r="G28" s="5">
+        <v>0.22631868418154735</v>
+      </c>
+      <c r="H28" s="5">
+        <v>0.5026639023247077</v>
+      </c>
+      <c r="J28" s="5">
+        <v>0.54815011861931962</v>
+      </c>
+      <c r="K28" s="5">
+        <v>0.4487476570841214</v>
+      </c>
+      <c r="L28" t="s">
+        <v>28</v>
+      </c>
+      <c r="N28" s="5">
+        <v>0.79224606407939746</v>
+      </c>
+      <c r="O28" s="5">
+        <v>0.12570635188470716</v>
+      </c>
+      <c r="P28" s="5">
+        <v>5.6547549085862431E-2</v>
+      </c>
+      <c r="R28" s="5">
+        <v>0.71916054760232295</v>
+      </c>
+      <c r="S28" s="5">
+        <v>0.23448899024174996</v>
+      </c>
+      <c r="T28" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>163</v>
+      </c>
+      <c r="B29" t="s">
+        <v>179</v>
+      </c>
+      <c r="C29" t="s">
+        <v>168</v>
+      </c>
+      <c r="D29" s="4">
+        <v>44478</v>
+      </c>
+      <c r="F29" s="5">
+        <v>0.3952386282899879</v>
+      </c>
+      <c r="G29" s="5">
+        <v>0.23508100890297004</v>
+      </c>
+      <c r="H29" s="5">
+        <v>0.34241071611319324</v>
+      </c>
+      <c r="J29" s="5">
+        <v>0.62114659169240538</v>
+      </c>
+      <c r="K29" s="5">
+        <v>0.37608309993786532</v>
+      </c>
+      <c r="L29" t="s">
+        <v>11</v>
+      </c>
+      <c r="N29" s="5">
+        <v>0.13615678302350348</v>
+      </c>
+      <c r="O29" s="5">
+        <v>0.45125858883215364</v>
+      </c>
+      <c r="P29" s="5">
+        <v>0.39124606391965616</v>
+      </c>
+      <c r="R29" s="5">
+        <v>7.8014599964736295E-2</v>
+      </c>
+      <c r="S29" s="5">
+        <v>0.92197645981455634</v>
+      </c>
+      <c r="T29" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>163</v>
+      </c>
+      <c r="B30" t="s">
+        <v>165</v>
+      </c>
+      <c r="C30" t="s">
+        <v>169</v>
+      </c>
+      <c r="D30" s="4">
+        <v>44478</v>
+      </c>
+      <c r="F30" s="5">
+        <v>0.51610431313037897</v>
+      </c>
+      <c r="G30" s="5">
+        <v>0.2405946890931171</v>
+      </c>
+      <c r="H30" s="5">
+        <v>0.23019521553312761</v>
+      </c>
+      <c r="J30" s="5">
+        <v>0.53449069432743779</v>
+      </c>
+      <c r="K30" s="5">
+        <v>0.46334768694931155</v>
+      </c>
+      <c r="L30" t="s">
+        <v>16</v>
+      </c>
+      <c r="N30" s="5">
+        <v>0.77724711890828269</v>
+      </c>
+      <c r="O30" s="5">
+        <v>0.10360606772035033</v>
+      </c>
+      <c r="P30" s="5">
+        <v>3.3189047532380167E-2</v>
+      </c>
+      <c r="R30" s="5">
+        <v>0.75011387925494732</v>
+      </c>
+      <c r="S30" s="5">
+        <v>0.12412264328540171</v>
+      </c>
+      <c r="T30" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>163</v>
+      </c>
+      <c r="B31" t="s">
+        <v>183</v>
+      </c>
+      <c r="C31" t="s">
+        <v>177</v>
+      </c>
+      <c r="D31" s="4">
+        <v>44478</v>
+      </c>
+      <c r="F31" s="5">
+        <v>0.34184607737586092</v>
+      </c>
+      <c r="G31" s="5">
+        <v>0.25898733172809707</v>
+      </c>
+      <c r="H31" s="5">
+        <v>0.36724857220515</v>
+      </c>
+      <c r="J31" s="5">
+        <v>0.50183438696515426</v>
+      </c>
+      <c r="K31" s="5">
+        <v>0.49716146765276142</v>
+      </c>
+      <c r="L31" t="s">
+        <v>20</v>
+      </c>
+      <c r="N31" s="5">
+        <v>0.18359793816774722</v>
+      </c>
+      <c r="O31" s="5">
+        <v>0.45260966598357666</v>
+      </c>
+      <c r="P31" s="5">
+        <v>0.34758776898437771</v>
+      </c>
+      <c r="R31" s="5">
+        <v>8.4462840960727287E-2</v>
+      </c>
+      <c r="S31" s="5">
+        <v>0.91553167427015325</v>
+      </c>
+      <c r="T31" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>163</v>
+      </c>
+      <c r="B32" t="s">
+        <v>379</v>
+      </c>
+      <c r="C32" t="s">
+        <v>173</v>
+      </c>
+      <c r="D32" s="4">
+        <v>44478</v>
+      </c>
+      <c r="F32" s="5">
+        <v>0.15777809274523852</v>
+      </c>
+      <c r="G32" s="5">
+        <v>0.26205167701182913</v>
+      </c>
+      <c r="H32" s="5">
+        <v>0.51335911970058801</v>
+      </c>
+      <c r="J32" s="5">
+        <v>0.35626610114841312</v>
+      </c>
+      <c r="K32" s="5">
+        <v>0.64283551689286</v>
+      </c>
+      <c r="L32" t="s">
+        <v>20</v>
+      </c>
+      <c r="N32" s="5">
+        <v>0.15386260651381758</v>
+      </c>
+      <c r="O32" s="5">
+        <v>0.30400243460623338</v>
+      </c>
+      <c r="P32" s="5">
+        <v>0.48737386312136954</v>
+      </c>
+      <c r="R32" s="5">
+        <v>0.25339631860570955</v>
+      </c>
+      <c r="S32" s="5">
+        <v>0.74631055336266705</v>
+      </c>
+      <c r="T32" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>163</v>
+      </c>
+      <c r="B33" t="s">
+        <v>187</v>
+      </c>
+      <c r="C33" t="s">
+        <v>164</v>
+      </c>
+      <c r="D33" s="4">
+        <v>44478</v>
+      </c>
+      <c r="F33" s="5">
+        <v>0.52739447478224466</v>
+      </c>
+      <c r="G33" s="5">
+        <v>0.26525062107391223</v>
+      </c>
+      <c r="H33" s="5">
+        <v>0.19848769587122544</v>
+      </c>
+      <c r="J33" s="5">
+        <v>0.40331679133830795</v>
+      </c>
+      <c r="K33" s="5">
+        <v>0.59579664591312154</v>
+      </c>
+      <c r="L33" t="s">
+        <v>20</v>
+      </c>
+      <c r="N33" s="5">
+        <v>0.15250005718674214</v>
+      </c>
+      <c r="O33" s="5">
+        <v>0.21225064156514306</v>
+      </c>
+      <c r="P33" s="5">
+        <v>0.55489845938357596</v>
+      </c>
+      <c r="R33" s="5">
+        <v>0.51810663647661548</v>
+      </c>
+      <c r="S33" s="5">
+        <v>0.47802814609838351</v>
+      </c>
+      <c r="T33" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>163</v>
+      </c>
+      <c r="B34" t="s">
+        <v>184</v>
+      </c>
+      <c r="C34" t="s">
+        <v>181</v>
+      </c>
+      <c r="D34" s="4">
+        <v>44478</v>
+      </c>
+      <c r="F34" s="5">
+        <v>0.22921340732597995</v>
+      </c>
+      <c r="G34" s="5">
+        <v>0.19244739789346402</v>
+      </c>
+      <c r="H34" s="5">
+        <v>0.51919971579434365</v>
+      </c>
+      <c r="J34" s="5">
+        <v>0.73076431001307485</v>
+      </c>
+      <c r="K34" s="5">
+        <v>0.25692058353951175</v>
+      </c>
+      <c r="L34" t="s">
+        <v>28</v>
+      </c>
+      <c r="N34" s="5">
+        <v>0.53252473284145352</v>
+      </c>
+      <c r="O34" s="5">
+        <v>0.41663279369263789</v>
+      </c>
+      <c r="P34" s="5">
+        <v>5.0725060151436671E-2</v>
+      </c>
+      <c r="R34" s="5">
+        <v>7.5976698757835082E-2</v>
+      </c>
+      <c r="S34" s="5">
+        <v>0.92399164787661969</v>
+      </c>
+      <c r="T34" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>163</v>
+      </c>
+      <c r="B35" t="s">
+        <v>182</v>
+      </c>
+      <c r="C35" t="s">
+        <v>186</v>
+      </c>
+      <c r="D35" s="4">
+        <v>44478</v>
+      </c>
+      <c r="F35" s="5">
+        <v>0.46990441382309034</v>
+      </c>
+      <c r="G35" s="5">
+        <v>0.24183727551044593</v>
+      </c>
+      <c r="H35" s="5">
+        <v>0.27049210004526458</v>
+      </c>
+      <c r="J35" s="5">
+        <v>0.56255848239114681</v>
+      </c>
+      <c r="K35" s="5">
+        <v>0.43533661599306972</v>
+      </c>
+      <c r="L35" t="s">
+        <v>16</v>
+      </c>
+      <c r="N35" s="5">
+        <v>0.47158112841299543</v>
+      </c>
+      <c r="O35" s="5">
+        <v>0.23672781974932641</v>
+      </c>
+      <c r="P35" s="5">
+        <v>0.27349141487387413</v>
+      </c>
+      <c r="R35" s="5">
+        <v>0.58927278742922606</v>
+      </c>
+      <c r="S35" s="5">
+        <v>0.40811768182421615</v>
+      </c>
+      <c r="T35" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>163</v>
+      </c>
+      <c r="B36" t="s">
+        <v>172</v>
+      </c>
+      <c r="C36" t="s">
+        <v>167</v>
+      </c>
+      <c r="D36" s="4">
+        <v>44478</v>
+      </c>
+      <c r="F36" s="5">
+        <v>0.32115878422038135</v>
+      </c>
+      <c r="G36" s="5">
+        <v>0.27425880272254205</v>
+      </c>
+      <c r="H36" s="5">
+        <v>0.37204208281151896</v>
+      </c>
+      <c r="J36" s="5">
+        <v>0.43513461379124141</v>
+      </c>
+      <c r="K36" s="5">
+        <v>0.56429819769247014</v>
+      </c>
+      <c r="L36" t="s">
+        <v>20</v>
+      </c>
+      <c r="N36" s="5">
+        <v>0.1236567108658836</v>
+      </c>
+      <c r="O36" s="5">
+        <v>0.33215301474359615</v>
+      </c>
+      <c r="P36" s="5">
+        <v>0.49258113394630165</v>
+      </c>
+      <c r="R36" s="5">
+        <v>0.18513451827235228</v>
+      </c>
+      <c r="S36" s="5">
+        <v>0.81471183428736382</v>
+      </c>
+      <c r="T36" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>381</v>
+      </c>
+      <c r="B37" t="s">
+        <v>394</v>
+      </c>
+      <c r="C37" t="s">
+        <v>386</v>
+      </c>
+      <c r="D37" s="4">
+        <v>44479</v>
+      </c>
+      <c r="F37" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G37" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H37" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J37" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K37" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L37" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="N37" s="5">
+        <v>0.15339944123370816</v>
+      </c>
+      <c r="O37" s="5">
+        <v>0.31560073799083854</v>
+      </c>
+      <c r="P37" s="5">
+        <v>0.47969192714236608</v>
+      </c>
+      <c r="R37" s="5">
+        <v>0.2313372730482405</v>
+      </c>
+      <c r="S37" s="5">
+        <v>0.76844435545030465</v>
+      </c>
+      <c r="T37" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>381</v>
+      </c>
+      <c r="B38" t="s">
+        <v>387</v>
+      </c>
+      <c r="C38" t="s">
+        <v>400</v>
+      </c>
+      <c r="D38" s="4">
+        <v>44479</v>
+      </c>
+      <c r="F38" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G38" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H38" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J38" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K38" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L38" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="N38" s="5">
+        <v>0.43758008034308765</v>
+      </c>
+      <c r="O38" s="5">
+        <v>0.21975742611605245</v>
+      </c>
+      <c r="P38" s="5">
+        <v>0.31883740508420944</v>
+      </c>
+      <c r="R38" s="5">
+        <v>0.69835720020897263</v>
+      </c>
+      <c r="S38" s="5">
+        <v>0.2959130257561684</v>
+      </c>
+      <c r="T38" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>381</v>
+      </c>
+      <c r="B39" t="s">
+        <v>391</v>
+      </c>
+      <c r="C39" t="s">
+        <v>382</v>
+      </c>
+      <c r="D39" s="4">
+        <v>44479</v>
+      </c>
+      <c r="F39" s="5">
+        <v>0.2991287320054894</v>
+      </c>
+      <c r="G39" s="5">
+        <v>0.31396652696431648</v>
+      </c>
+      <c r="H39" s="5">
+        <v>0.35905576543477635</v>
+      </c>
+      <c r="J39" s="5">
+        <v>0.30378668446852058</v>
+      </c>
+      <c r="K39" s="5">
+        <v>0.69606503595092417</v>
+      </c>
+      <c r="L39" t="s">
+        <v>20</v>
+      </c>
+      <c r="N39" s="5">
+        <v>0.53688624212051028</v>
+      </c>
+      <c r="O39" s="5">
+        <v>0.34904085121532191</v>
+      </c>
+      <c r="P39" s="5">
+        <v>0.11266636563348763</v>
+      </c>
+      <c r="R39" s="5">
+        <v>0.15814959193833769</v>
+      </c>
+      <c r="S39" s="5">
+        <v>0.84174349146703165</v>
+      </c>
+      <c r="T39" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>381</v>
+      </c>
+      <c r="B40" t="s">
+        <v>392</v>
+      </c>
+      <c r="C40" t="s">
+        <v>398</v>
+      </c>
+      <c r="D40" s="4">
+        <v>44479</v>
+      </c>
+      <c r="F40" s="5">
+        <v>0.55338131653275136</v>
+      </c>
+      <c r="G40" s="5">
+        <v>0.30483718705406992</v>
+      </c>
+      <c r="H40" s="5">
+        <v>0.13872584699022281</v>
+      </c>
+      <c r="J40" s="5">
+        <v>0.24297124573161097</v>
+      </c>
+      <c r="K40" s="5">
+        <v>0.75673613782579585</v>
+      </c>
+      <c r="L40" t="s">
+        <v>17</v>
+      </c>
+      <c r="N40" s="5">
+        <v>0.15581995133375071</v>
+      </c>
+      <c r="O40" s="5">
+        <v>0.46169239652634297</v>
+      </c>
+      <c r="P40" s="5">
+        <v>0.36489583869792586</v>
+      </c>
+      <c r="R40" s="5">
+        <v>7.4883359306565381E-2</v>
+      </c>
+      <c r="S40" s="5">
+        <v>0.92511090640812754</v>
+      </c>
+      <c r="T40" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>381</v>
+      </c>
+      <c r="B41" t="s">
+        <v>383</v>
+      </c>
+      <c r="C41" t="s">
+        <v>384</v>
+      </c>
+      <c r="D41" s="4">
+        <v>44479</v>
+      </c>
+      <c r="F41" s="5">
+        <v>0.72274103846890403</v>
+      </c>
+      <c r="G41" s="5">
+        <v>0.1892022355254325</v>
+      </c>
+      <c r="H41" s="5">
+        <v>8.5093986531056098E-2</v>
+      </c>
+      <c r="J41" s="5">
+        <v>0.47340932798595503</v>
+      </c>
+      <c r="K41" s="5">
+        <v>0.52150269685107986</v>
+      </c>
+      <c r="L41" t="s">
+        <v>16</v>
+      </c>
+      <c r="N41" s="5">
+        <v>0.82340548451526019</v>
+      </c>
+      <c r="O41" s="5">
+        <v>0.13292884826027146</v>
+      </c>
+      <c r="P41" s="5">
+        <v>3.7062004531528636E-2</v>
+      </c>
+      <c r="R41" s="5">
+        <v>0.51272247209421873</v>
+      </c>
+      <c r="S41" s="5">
+        <v>0.4749313460008962</v>
+      </c>
+      <c r="T41" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>381</v>
+      </c>
+      <c r="B42" t="s">
+        <v>389</v>
+      </c>
+      <c r="C42" t="s">
+        <v>390</v>
+      </c>
+      <c r="D42" s="4">
+        <v>44479</v>
+      </c>
+      <c r="F42" s="5">
+        <v>0.30308564740960858</v>
+      </c>
+      <c r="G42" s="5">
+        <v>0.31295383328912751</v>
+      </c>
+      <c r="H42" s="5">
+        <v>0.35646290592088026</v>
+      </c>
+      <c r="J42" s="5">
+        <v>0.30722236584920198</v>
+      </c>
+      <c r="K42" s="5">
+        <v>0.69262577554096372</v>
+      </c>
+      <c r="L42" t="s">
+        <v>20</v>
+      </c>
+      <c r="N42" s="5">
+        <v>0.41419120119995556</v>
+      </c>
+      <c r="O42" s="5">
+        <v>0.29066803609204456</v>
+      </c>
+      <c r="P42" s="5">
+        <v>0.2779890157199284</v>
+      </c>
+      <c r="R42" s="5">
+        <v>0.37161383934803116</v>
+      </c>
+      <c r="S42" s="5">
+        <v>0.62805479696218613</v>
+      </c>
+      <c r="T42" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>381</v>
+      </c>
+      <c r="B43" t="s">
+        <v>403</v>
+      </c>
+      <c r="C43" t="s">
+        <v>388</v>
+      </c>
+      <c r="D43" s="4">
+        <v>44479</v>
+      </c>
+      <c r="F43" s="5">
+        <v>0.27299898801163874</v>
+      </c>
+      <c r="G43" s="5">
+        <v>0.29891892320810948</v>
+      </c>
+      <c r="H43" s="5">
+        <v>0.39303045825467509</v>
+      </c>
+      <c r="J43" s="5">
+        <v>0.33787052198277223</v>
+      </c>
+      <c r="K43" s="5">
+        <v>0.66186803906782288</v>
+      </c>
+      <c r="L43" t="s">
+        <v>20</v>
+      </c>
+      <c r="N43" s="5">
+        <v>0.83075866570753099</v>
+      </c>
+      <c r="O43" s="5">
+        <v>0.12350139152701065</v>
+      </c>
+      <c r="P43" s="5">
+        <v>3.6367986736746342E-2</v>
+      </c>
+      <c r="R43" s="5">
+        <v>0.55741912520627257</v>
+      </c>
+      <c r="S43" s="5">
+        <v>0.42527842842769104</v>
+      </c>
+      <c r="T43" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>381</v>
+      </c>
+      <c r="B44" t="s">
+        <v>395</v>
+      </c>
+      <c r="C44" t="s">
+        <v>402</v>
+      </c>
+      <c r="D44" s="4">
+        <v>44479</v>
+      </c>
+      <c r="F44" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G44" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H44" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J44" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K44" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L44" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="N44" s="5">
+        <v>0.34873053012592714</v>
+      </c>
+      <c r="O44" s="5">
+        <v>0.37821951158757755</v>
+      </c>
+      <c r="P44" s="5">
+        <v>0.2621436105284391</v>
+      </c>
+      <c r="R44" s="5">
+        <v>0.17194212406494039</v>
+      </c>
+      <c r="S44" s="5">
+        <v>0.82803555085124503</v>
+      </c>
+      <c r="T44" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>381</v>
+      </c>
+      <c r="B45" t="s">
+        <v>399</v>
+      </c>
+      <c r="C45" t="s">
+        <v>396</v>
+      </c>
+      <c r="D45" s="4">
+        <v>44479</v>
+      </c>
+      <c r="F45" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G45" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H45" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J45" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K45" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L45" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="N45" s="5">
+        <v>0.64521921174221353</v>
+      </c>
+      <c r="O45" s="5">
+        <v>0.31509799560693158</v>
+      </c>
+      <c r="P45" s="5">
+        <v>3.949685168955952E-2</v>
+      </c>
+      <c r="R45" s="5">
+        <v>0.1423224980390542</v>
+      </c>
+      <c r="S45" s="5">
+        <v>0.85745961388356395</v>
+      </c>
+      <c r="T45" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>381</v>
+      </c>
+      <c r="B46" t="s">
+        <v>393</v>
+      </c>
+      <c r="C46" t="s">
+        <v>397</v>
+      </c>
+      <c r="D46" s="4">
+        <v>44479</v>
+      </c>
+      <c r="F46" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G46" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H46" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J46" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K46" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L46" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="N46" s="5">
+        <v>0.4633897413816459</v>
+      </c>
+      <c r="O46" s="5">
+        <v>0.35645426453590584</v>
+      </c>
+      <c r="P46" s="5">
+        <v>0.17573592144216749</v>
+      </c>
+      <c r="R46" s="5">
+        <v>0.18080091069245849</v>
+      </c>
+      <c r="S46" s="5">
+        <v>0.81912854491202081</v>
+      </c>
+      <c r="T46" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>381</v>
+      </c>
+      <c r="B47" t="s">
+        <v>385</v>
+      </c>
+      <c r="C47" t="s">
+        <v>401</v>
+      </c>
+      <c r="D47" s="4">
+        <v>44479</v>
+      </c>
+      <c r="F47" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G47" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H47" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J47" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K47" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L47" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="N47" s="5">
+        <v>0.42305633038621199</v>
+      </c>
+      <c r="O47" s="5">
+        <v>0.27888565589335468</v>
+      </c>
+      <c r="P47" s="5">
+        <v>0.28008397774977911</v>
+      </c>
+      <c r="R47" s="5">
+        <v>0.4127451348768203</v>
+      </c>
+      <c r="S47" s="5">
+        <v>0.58675403393741055</v>
+      </c>
+      <c r="T47" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updated weekend fixtures for 18/10/2021
</commit_message>
<xml_diff>
--- a/picks.xlsx
+++ b/picks.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2992" uniqueCount="411">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3004" uniqueCount="411">
   <si>
     <t>Div</t>
   </si>
@@ -22700,13 +22700,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T155"/>
+  <dimension ref="A1:T180"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A8" sqref="A8:XFD8"/>
+      <selection pane="bottomRight" activeCell="A16" sqref="A16:XFD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22776,22 +22776,22 @@
         <v>44484</v>
       </c>
       <c r="F2" s="5">
-        <v>0.60343711786356957</v>
+        <v>0.39183356415571163</v>
       </c>
       <c r="G2" s="5">
-        <v>0.31054824362952288</v>
+        <v>0.24764030599254036</v>
       </c>
       <c r="H2" s="5">
-        <v>8.5191792406568392E-2</v>
+        <v>0.33414340014276528</v>
       </c>
       <c r="J2" s="5">
-        <v>0.18660137199687762</v>
+        <v>0.5577885621618528</v>
       </c>
       <c r="K2" s="5">
-        <v>0.8131447260982807</v>
+        <v>0.44060326061017874</v>
       </c>
       <c r="L2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="N2" s="5">
         <v>0.60343711786356957</v>
@@ -22826,19 +22826,19 @@
         <v>44484</v>
       </c>
       <c r="F3" s="5">
-        <v>0.22261608782664832</v>
+        <v>0.48360959398996978</v>
       </c>
       <c r="G3" s="5">
-        <v>0.34391241631656078</v>
+        <v>0.29015949775404387</v>
       </c>
       <c r="H3" s="5">
-        <v>0.40118037338579121</v>
+        <v>0.21640717463473605</v>
       </c>
       <c r="J3" s="5">
-        <v>0.21667913733688424</v>
+        <v>0.34067377834963475</v>
       </c>
       <c r="K3" s="5">
-        <v>0.78324075501529078</v>
+        <v>0.65893157889167497</v>
       </c>
       <c r="L3" t="s">
         <v>20</v>
@@ -22876,19 +22876,19 @@
         <v>44484</v>
       </c>
       <c r="F4" s="5">
-        <v>0.44045832869799917</v>
+        <v>0.59069354995629031</v>
       </c>
       <c r="G4" s="5">
-        <v>0.25483061835853044</v>
+        <v>0.23460692961471988</v>
       </c>
       <c r="H4" s="5">
-        <v>0.28527106932953356</v>
+        <v>0.16772670521575628</v>
       </c>
       <c r="J4" s="5">
-        <v>0.51125197264456779</v>
+        <v>0.47751013190259756</v>
       </c>
       <c r="K4" s="5">
-        <v>0.48751225391426661</v>
+        <v>0.5202031678137643</v>
       </c>
       <c r="L4" t="s">
         <v>16</v>
@@ -22926,22 +22926,22 @@
         <v>44484</v>
       </c>
       <c r="F5" s="5">
-        <v>0.62532796652584044</v>
+        <v>0.22915301338892213</v>
       </c>
       <c r="G5" s="5">
-        <v>0.33431049872252544</v>
+        <v>0.24338831724184884</v>
       </c>
       <c r="H5" s="5">
-        <v>4.0211920855203594E-2</v>
+        <v>0.47277331998129757</v>
       </c>
       <c r="J5" s="5">
-        <v>0.12590707996953149</v>
+        <v>0.50002288774577131</v>
       </c>
       <c r="K5" s="5">
-        <v>0.87394048128276924</v>
+        <v>0.49819401619550285</v>
       </c>
       <c r="L5" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="N5" s="5">
         <v>0.62532796652584044</v>
@@ -22976,22 +22976,22 @@
         <v>44484</v>
       </c>
       <c r="F6" s="5">
-        <v>0.73874553877782378</v>
+        <v>0.53643229340418508</v>
       </c>
       <c r="G6" s="5">
-        <v>0.23322147230051393</v>
+        <v>0.21908077293227446</v>
       </c>
       <c r="H6" s="5">
-        <v>2.7399386180147121E-2</v>
+        <v>0.23046237267505446</v>
       </c>
       <c r="J6" s="5">
-        <v>0.22413470628311896</v>
+        <v>0.64073980539030573</v>
       </c>
       <c r="K6" s="5">
-        <v>0.77489759493393984</v>
+        <v>0.35402096087676016</v>
       </c>
       <c r="L6" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
       <c r="N6" s="5">
         <v>0.73874553877782378</v>
@@ -23026,22 +23026,22 @@
         <v>44484</v>
       </c>
       <c r="F7" s="5">
-        <v>0.38018996081071232</v>
+        <v>0.37472194528908298</v>
       </c>
       <c r="G7" s="5">
-        <v>0.41519499829250678</v>
+        <v>0.26271398094452703</v>
       </c>
       <c r="H7" s="5">
-        <v>0.19981922326030785</v>
+        <v>0.33590245484936537</v>
       </c>
       <c r="J7" s="5">
-        <v>0.11810396398675804</v>
+        <v>0.48875182981372439</v>
       </c>
       <c r="K7" s="5">
-        <v>0.88188358155290647</v>
+        <v>0.51037944663615975</v>
       </c>
       <c r="L7" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="N7" s="5">
         <v>0.38018996081071232</v>
@@ -23076,22 +23076,22 @@
         <v>44484</v>
       </c>
       <c r="F8" s="5">
-        <v>0.29068137273338657</v>
+        <v>0.31931467627513987</v>
       </c>
       <c r="G8" s="5">
-        <v>0.2205780115876633</v>
+        <v>0.21802664708218275</v>
       </c>
       <c r="H8" s="5">
-        <v>0.44438638207687431</v>
+        <v>0.42314854881637276</v>
       </c>
       <c r="J8" s="5">
-        <v>0.65762976433362863</v>
+        <v>0.68873105292111847</v>
       </c>
       <c r="K8" s="5">
-        <v>0.33765391183037458</v>
+        <v>0.30570982699893345</v>
       </c>
       <c r="L8" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="N8" s="5">
         <v>0.29068137273338657</v>
@@ -23126,22 +23126,22 @@
         <v>44484</v>
       </c>
       <c r="F9" s="5">
-        <v>0.62821148950907857</v>
+        <v>0.58011223053870731</v>
       </c>
       <c r="G9" s="5">
-        <v>0.27423316465649117</v>
+        <v>0.24124201065090231</v>
       </c>
       <c r="H9" s="5">
-        <v>9.6140188756918626E-2</v>
+        <v>0.17156371929812428</v>
       </c>
       <c r="J9" s="5">
-        <v>0.25658740333065655</v>
+        <v>0.45703786681950287</v>
       </c>
       <c r="K9" s="5">
-        <v>0.7428289570007155</v>
+        <v>0.54110551674667673</v>
       </c>
       <c r="L9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="N9" s="5">
         <v>0.62821148950907857</v>
@@ -23176,19 +23176,19 @@
         <v>44484</v>
       </c>
       <c r="F10" s="5">
-        <v>0.6748129659307146</v>
+        <v>0.64777369292940268</v>
       </c>
       <c r="G10" s="5">
-        <v>0.20875507449677436</v>
+        <v>0.20143081685967387</v>
       </c>
       <c r="H10" s="5">
-        <v>0.11277840797770244</v>
+        <v>0.14398594098672016</v>
       </c>
       <c r="J10" s="5">
-        <v>0.47136928479296464</v>
+        <v>0.5831193858992697</v>
       </c>
       <c r="K10" s="5">
-        <v>0.5249011841947786</v>
+        <v>0.41034845793837127</v>
       </c>
       <c r="L10" t="s">
         <v>16</v>
@@ -23226,19 +23226,19 @@
         <v>44485</v>
       </c>
       <c r="F11" s="5">
-        <v>0.17219478915125211</v>
+        <v>0.30534181714234476</v>
       </c>
       <c r="G11" s="5">
-        <v>0.27702680612850455</v>
+        <v>0.2834500122814102</v>
       </c>
       <c r="H11" s="5">
-        <v>0.4915728102302141</v>
+        <v>0.37797101276420891</v>
       </c>
       <c r="J11" s="5">
-        <v>0.33105623945565155</v>
+        <v>0.39760719361878472</v>
       </c>
       <c r="K11" s="5">
-        <v>0.66834402479577948</v>
+        <v>0.60197821774901494</v>
       </c>
       <c r="L11" t="s">
         <v>20</v>
@@ -23276,22 +23276,22 @@
         <v>44485</v>
       </c>
       <c r="F12" s="5">
-        <v>7.0363012409525333E-2</v>
+        <v>0.16761108138414402</v>
       </c>
       <c r="G12" s="5">
-        <v>9.2605542482924103E-2</v>
+        <v>0.17985322485952612</v>
       </c>
       <c r="H12" s="5">
-        <v>0.67646782873513145</v>
+        <v>0.57479397454695069</v>
       </c>
       <c r="J12" s="5">
-        <v>0.78544066382908773</v>
+        <v>0.69179589543261089</v>
       </c>
       <c r="K12" s="5">
-        <v>0.11159134588826017</v>
+        <v>0.29492011302575916</v>
       </c>
       <c r="L12" t="s">
-        <v>170</v>
+        <v>28</v>
       </c>
       <c r="N12" s="5">
         <v>7.0363012409525333E-2</v>
@@ -23326,22 +23326,22 @@
         <v>44485</v>
       </c>
       <c r="F13" s="5">
-        <v>0.24999777347848839</v>
+        <v>0.63131437495314924</v>
       </c>
       <c r="G13" s="5">
-        <v>0.24672526523215549</v>
+        <v>0.22229007728424829</v>
       </c>
       <c r="H13" s="5">
-        <v>0.45353273941836697</v>
+        <v>0.1412111746561551</v>
       </c>
       <c r="J13" s="5">
-        <v>0.50580818133213645</v>
+        <v>0.47991823857455229</v>
       </c>
       <c r="K13" s="5">
-        <v>0.49257744274635085</v>
+        <v>0.51707743776356074</v>
       </c>
       <c r="L13" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="N13" s="5">
         <v>0.24999777347848839</v>
@@ -23376,22 +23376,22 @@
         <v>44485</v>
       </c>
       <c r="F14" s="5">
-        <v>0.27406376975095448</v>
+        <v>0.51704462757902148</v>
       </c>
       <c r="G14" s="5">
-        <v>0.19092007015607676</v>
+        <v>0.24924245425350311</v>
       </c>
       <c r="H14" s="5">
-        <v>0.48439803128633813</v>
+        <v>0.22181440200283206</v>
       </c>
       <c r="J14" s="5">
-        <v>0.78472492756857337</v>
+        <v>0.48814033104369697</v>
       </c>
       <c r="K14" s="5">
-        <v>0.19875879950695519</v>
+        <v>0.51030905020381534</v>
       </c>
       <c r="L14" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="N14" s="5">
         <v>0.27406376975095448</v>
@@ -23426,22 +23426,22 @@
         <v>44485</v>
       </c>
       <c r="F15" s="5">
-        <v>0.4118980015520361</v>
+        <v>0.36056681667883489</v>
       </c>
       <c r="G15" s="5">
-        <v>0.24694241549553786</v>
+        <v>0.28836198855153766</v>
       </c>
       <c r="H15" s="5">
-        <v>0.3172609790703701</v>
+        <v>0.32676336157270808</v>
       </c>
       <c r="J15" s="5">
-        <v>0.55862582539624772</v>
+        <v>0.38821264984440956</v>
       </c>
       <c r="K15" s="5">
-        <v>0.43970265045937895</v>
+        <v>0.61145324866220852</v>
       </c>
       <c r="L15" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="N15" s="5">
         <v>0.4118980015520361</v>
@@ -23476,19 +23476,19 @@
         <v>44485</v>
       </c>
       <c r="F16" s="5">
-        <v>0.51638748816665014</v>
+        <v>0.6024287279824776</v>
       </c>
       <c r="G16" s="5">
-        <v>0.25772418184008367</v>
+        <v>0.24068953948754687</v>
       </c>
       <c r="H16" s="5">
-        <v>0.21502331627365442</v>
+        <v>0.15152334451225205</v>
       </c>
       <c r="J16" s="5">
-        <v>0.44736586482658558</v>
+        <v>0.42767592888329858</v>
       </c>
       <c r="K16" s="5">
-        <v>0.55149006100394515</v>
+        <v>0.5705695067478056</v>
       </c>
       <c r="L16" t="s">
         <v>16</v>
@@ -23526,22 +23526,22 @@
         <v>44485</v>
       </c>
       <c r="F17" s="5">
-        <v>0</v>
+        <v>0.38297037226912189</v>
       </c>
       <c r="G17" s="5">
-        <v>0.24930455935293025</v>
+        <v>0.22618498946750237</v>
       </c>
       <c r="H17" s="5">
-        <v>0.63873270230865931</v>
+        <v>0.36120369650425843</v>
       </c>
       <c r="J17" s="5">
-        <v>0.16327484403996767</v>
+        <v>0.66745456721898633</v>
       </c>
       <c r="K17" s="5">
-        <v>0.83613050105698772</v>
+        <v>0.32842102338741758</v>
       </c>
       <c r="L17" t="s">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="N17" s="5">
         <v>0</v>
@@ -23576,22 +23576,22 @@
         <v>44485</v>
       </c>
       <c r="F18" s="5">
-        <v>0.44809820780076659</v>
+        <v>0.52220846647255781</v>
       </c>
       <c r="G18" s="5">
-        <v>0.28536535599958324</v>
+        <v>0.21507597136800674</v>
       </c>
       <c r="H18" s="5">
-        <v>0.25241002367920029</v>
+        <v>0.2466700552581447</v>
       </c>
       <c r="J18" s="5">
-        <v>0.37778817590327579</v>
+        <v>0.67938215536729762</v>
       </c>
       <c r="K18" s="5">
-        <v>0.62178790671182127</v>
+        <v>0.31403950427389105</v>
       </c>
       <c r="L18" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="N18" s="5">
         <v>0.44809820780076659</v>
@@ -23625,23 +23625,23 @@
       <c r="D19" s="4">
         <v>44485</v>
       </c>
-      <c r="F19" s="5">
-        <v>0.84078911974821691</v>
-      </c>
-      <c r="G19" s="5">
-        <v>0.12086228883355049</v>
-      </c>
-      <c r="H19" s="5">
-        <v>2.9723591153163791E-2</v>
-      </c>
-      <c r="J19" s="5">
-        <v>0.52258014208327308</v>
-      </c>
-      <c r="K19" s="5">
-        <v>0.46260111849024976</v>
-      </c>
-      <c r="L19" t="s">
-        <v>21</v>
+      <c r="F19" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G19" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H19" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J19" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K19" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L19" t="e">
+        <v>#N/A</v>
       </c>
       <c r="N19" s="5">
         <v>0.84078911974821691</v>
@@ -23676,22 +23676,22 @@
         <v>44485</v>
       </c>
       <c r="F20" s="5">
-        <v>6.30287727518066E-2</v>
+        <v>0.54870394340998641</v>
       </c>
       <c r="G20" s="5">
-        <v>0.10286929153206191</v>
+        <v>0.23628054029294399</v>
       </c>
       <c r="H20" s="5">
-        <v>0.69021617715866745</v>
+        <v>0.20451290400326924</v>
       </c>
       <c r="J20" s="5">
-        <v>0.74082784912740118</v>
+        <v>0.52419324455117056</v>
       </c>
       <c r="K20" s="5">
-        <v>0.20520356080923327</v>
+        <v>0.47337599861422042</v>
       </c>
       <c r="L20" t="s">
-        <v>72</v>
+        <v>16</v>
       </c>
       <c r="N20" s="5">
         <v>6.30287727518066E-2</v>
@@ -23726,22 +23726,22 @@
         <v>44485</v>
       </c>
       <c r="F21" s="5">
-        <v>0.29779607501477884</v>
+        <v>0.55399703896669217</v>
       </c>
       <c r="G21" s="5">
-        <v>0.56823811674059976</v>
+        <v>0.25135106316412564</v>
       </c>
       <c r="H21" s="5">
-        <v>0.13303544773689996</v>
+        <v>0.18650403323048631</v>
       </c>
       <c r="J21" s="5">
-        <v>2.9456135381231086E-2</v>
+        <v>0.4391565672279476</v>
       </c>
       <c r="K21" s="5">
-        <v>0.970543435908513</v>
+        <v>0.55946381164183578</v>
       </c>
       <c r="L21" t="s">
-        <v>133</v>
+        <v>16</v>
       </c>
       <c r="N21" s="5">
         <v>0.29779607501477884</v>
@@ -23776,22 +23776,22 @@
         <v>44485</v>
       </c>
       <c r="F22" s="5">
-        <v>0.17513513986578741</v>
+        <v>0.18611786760503776</v>
       </c>
       <c r="G22" s="5">
-        <v>0.37822240423426429</v>
+        <v>0.20041599868619078</v>
       </c>
       <c r="H22" s="5">
-        <v>0.4155318420712909</v>
+        <v>0.54284900123347368</v>
       </c>
       <c r="J22" s="5">
-        <v>0.1505332496513089</v>
+        <v>0.62976704937153438</v>
       </c>
       <c r="K22" s="5">
-        <v>0.84942556776645373</v>
+        <v>0.36316641991862042</v>
       </c>
       <c r="L22" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="N22" s="5">
         <v>0.17513513986578741</v>
@@ -23826,22 +23826,22 @@
         <v>44485</v>
       </c>
       <c r="F23" s="5">
-        <v>0.72763539713243452</v>
+        <v>0.75551689376595121</v>
       </c>
       <c r="G23" s="5">
-        <v>5.5453252691467832E-3</v>
+        <v>0.15981634585860857</v>
       </c>
       <c r="H23" s="5">
-        <v>0</v>
+        <v>7.8324196139920255E-2</v>
       </c>
       <c r="J23" s="5">
-        <v>0.62400561440788638</v>
+        <v>0.59255235236764192</v>
       </c>
       <c r="K23" s="5">
-        <v>0.10917510799369491</v>
+        <v>0.39418524592804838</v>
       </c>
       <c r="L23" t="s">
-        <v>83</v>
+        <v>16</v>
       </c>
       <c r="N23" s="5">
         <v>0.72763539713243452</v>
@@ -23876,22 +23876,22 @@
         <v>44485</v>
       </c>
       <c r="F24" s="5">
-        <v>3.221312152209483E-2</v>
+        <v>0.64605972320972427</v>
       </c>
       <c r="G24" s="5">
-        <v>0.12706516039200291</v>
+        <v>0.23165086612685576</v>
       </c>
       <c r="H24" s="5">
-        <v>0.67475631948025017</v>
+        <v>0.11903644202262148</v>
       </c>
       <c r="J24" s="5">
-        <v>0.48555372998232199</v>
+        <v>0.40098870639285283</v>
       </c>
       <c r="K24" s="5">
-        <v>0.50357725027246614</v>
+        <v>0.59706435145402792</v>
       </c>
       <c r="L24" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="N24" s="5">
         <v>3.221312152209483E-2</v>
@@ -23926,22 +23926,22 @@
         <v>44485</v>
       </c>
       <c r="F25" s="5">
-        <v>0.28486374811667503</v>
+        <v>0.41573475751070638</v>
       </c>
       <c r="G25" s="5">
-        <v>0.47469566319127526</v>
+        <v>0.22015198535912089</v>
       </c>
       <c r="H25" s="5">
-        <v>0.23467006085490311</v>
+        <v>0.33790027625149194</v>
       </c>
       <c r="J25" s="5">
-        <v>7.3864042826278675E-2</v>
+        <v>0.69983567615649567</v>
       </c>
       <c r="K25" s="5">
-        <v>0.92613424585256454</v>
+        <v>0.29456858391028568</v>
       </c>
       <c r="L25" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="N25" s="5">
         <v>0.28486374811667503</v>
@@ -23976,22 +23976,22 @@
         <v>44485</v>
       </c>
       <c r="F26" s="5">
-        <v>6.9888318945075259E-2</v>
+        <v>0.39059025481581</v>
       </c>
       <c r="G26" s="5">
-        <v>0.20796311202971982</v>
+        <v>0.27314377490677316</v>
       </c>
       <c r="H26" s="5">
-        <v>0.61064641851981927</v>
+        <v>0.31334246647112773</v>
       </c>
       <c r="J26" s="5">
-        <v>0.35787772293918735</v>
+        <v>0.4435418782590701</v>
       </c>
       <c r="K26" s="5">
-        <v>0.63977721096281559</v>
+        <v>0.55586849997095877</v>
       </c>
       <c r="L26" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="N26" s="5">
         <v>6.9888318945075259E-2</v>
@@ -24026,22 +24026,22 @@
         <v>44485</v>
       </c>
       <c r="F27" s="5">
-        <v>0.86333862472608214</v>
+        <v>0.64624775523403488</v>
       </c>
       <c r="G27" s="5">
-        <v>9.0459991957449651E-2</v>
+        <v>0.19978154311746482</v>
       </c>
       <c r="H27" s="5">
-        <v>2.1103746296397084E-2</v>
+        <v>0.14670079174222361</v>
       </c>
       <c r="J27" s="5">
-        <v>0.62953482569546293</v>
+        <v>0.59839650789379395</v>
       </c>
       <c r="K27" s="5">
-        <v>0.332055339181973</v>
+        <v>0.39443870217449262</v>
       </c>
       <c r="L27" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="N27" s="5">
         <v>0.86333862472608214</v>
@@ -24076,22 +24076,22 @@
         <v>44485</v>
       </c>
       <c r="F28" s="5">
-        <v>4.6508964093147503E-2</v>
+        <v>0.11972082182807456</v>
       </c>
       <c r="G28" s="5">
-        <v>0.54414123277521076</v>
+        <v>0.22212454855829691</v>
       </c>
       <c r="H28" s="5">
-        <v>0.3931550111000936</v>
+        <v>0.56913155568496587</v>
       </c>
       <c r="J28" s="5">
-        <v>2.9004342076063585E-2</v>
+        <v>0.42001351074711929</v>
       </c>
       <c r="K28" s="5">
-        <v>0.97099324120563046</v>
+        <v>0.57762715681483634</v>
       </c>
       <c r="L28" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="N28" s="5">
         <v>4.6508964093147503E-2</v>
@@ -24126,22 +24126,22 @@
         <v>44485</v>
       </c>
       <c r="F29" s="5">
-        <v>0.64162425320815963</v>
+        <v>0.13222212814965686</v>
       </c>
       <c r="G29" s="5">
-        <v>0.18478960259610916</v>
+        <v>0.31221555714549598</v>
       </c>
       <c r="H29" s="5">
-        <v>0.16073593826782995</v>
+        <v>0.49924121032123198</v>
       </c>
       <c r="J29" s="5">
-        <v>0.71880297101638346</v>
+        <v>0.22152221096951122</v>
       </c>
       <c r="K29" s="5">
-        <v>0.26459835284507238</v>
+        <v>0.77823439551971951</v>
       </c>
       <c r="L29" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="N29" s="5">
         <v>0.64162425320815963</v>
@@ -24176,22 +24176,22 @@
         <v>44485</v>
       </c>
       <c r="F30" s="5">
-        <v>0.55273215868993397</v>
+        <v>0.2165481723066483</v>
       </c>
       <c r="G30" s="5">
-        <v>0.23385297801217592</v>
+        <v>0.24637601472252291</v>
       </c>
       <c r="H30" s="5">
-        <v>0.20297662192479199</v>
+        <v>0.4801061612019013</v>
       </c>
       <c r="J30" s="5">
-        <v>0.53314860466817282</v>
+        <v>0.47523259437045168</v>
       </c>
       <c r="K30" s="5">
-        <v>0.46420013848238956</v>
+        <v>0.52318239004604195</v>
       </c>
       <c r="L30" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="N30" s="5">
         <v>0.55273215868993397</v>
@@ -24226,22 +24226,22 @@
         <v>44485</v>
       </c>
       <c r="F31" s="5">
-        <v>0.82578373742655597</v>
+        <v>0.31754188068411821</v>
       </c>
       <c r="G31" s="5">
-        <v>9.4853108978377176E-2</v>
+        <v>0.29374885602755352</v>
       </c>
       <c r="H31" s="5">
-        <v>2.704162943476391E-2</v>
+        <v>0.35936954401246202</v>
       </c>
       <c r="J31" s="5">
-        <v>0.72085148183788972</v>
+        <v>0.36629959986111937</v>
       </c>
       <c r="K31" s="5">
-        <v>0.19847950776209081</v>
+        <v>0.63341710878676727</v>
       </c>
       <c r="L31" t="s">
-        <v>47</v>
+        <v>20</v>
       </c>
       <c r="N31" s="5">
         <v>0.82578373742655597</v>
@@ -24276,19 +24276,19 @@
         <v>44485</v>
       </c>
       <c r="F32" s="5">
-        <v>0.45467110581539621</v>
+        <v>0.43614403746370678</v>
       </c>
       <c r="G32" s="5">
-        <v>0.27266575517592717</v>
+        <v>0.32791028886213786</v>
       </c>
       <c r="H32" s="5">
-        <v>0.25738959056373523</v>
+        <v>0.2265385154230051</v>
       </c>
       <c r="J32" s="5">
-        <v>0.42451532507445772</v>
+        <v>0.25279352515832981</v>
       </c>
       <c r="K32" s="5">
-        <v>0.57483149821227708</v>
+        <v>0.74708572472606993</v>
       </c>
       <c r="L32" t="s">
         <v>20</v>
@@ -24326,22 +24326,22 @@
         <v>44485</v>
       </c>
       <c r="F33" s="5">
-        <v>0.16133914278995579</v>
+        <v>0.19110523209693647</v>
       </c>
       <c r="G33" s="5">
-        <v>0.22677401008334933</v>
+        <v>0.33240917529111036</v>
       </c>
       <c r="H33" s="5">
-        <v>0.53695910440212224</v>
+        <v>0.43644413466437776</v>
       </c>
       <c r="J33" s="5">
-        <v>0.47672481860484073</v>
+        <v>0.22385080202264598</v>
       </c>
       <c r="K33" s="5">
-        <v>0.52071418671560876</v>
+        <v>0.77602220337402894</v>
       </c>
       <c r="L33" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="N33" s="5">
         <v>0.16133914278995579</v>
@@ -24376,22 +24376,22 @@
         <v>44485</v>
       </c>
       <c r="F34" s="5">
-        <v>0.49801047528008896</v>
+        <v>0.42418820154239362</v>
       </c>
       <c r="G34" s="5">
-        <v>0.35442213786700405</v>
+        <v>0.33361167935851366</v>
       </c>
       <c r="H34" s="5">
-        <v>0.14487437632105674</v>
+        <v>0.23242755056214293</v>
       </c>
       <c r="J34" s="5">
-        <v>0.16909172358795815</v>
+        <v>0.24321750951703694</v>
       </c>
       <c r="K34" s="5">
-        <v>0.8308229012844317</v>
+        <v>0.75668351610996598</v>
       </c>
       <c r="L34" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="N34" s="5">
         <v>0.49801047528008896</v>
@@ -24426,22 +24426,22 @@
         <v>44485</v>
       </c>
       <c r="F35" s="5">
-        <v>0.70985736149037348</v>
+        <v>0.42313174839009399</v>
       </c>
       <c r="G35" s="5">
-        <v>0.17153032266997359</v>
+        <v>0.24686843957037113</v>
       </c>
       <c r="H35" s="5">
-        <v>0.11006908532076436</v>
+        <v>0.30747353878212674</v>
       </c>
       <c r="J35" s="5">
-        <v>0.65371776573067319</v>
+        <v>0.55637522405697803</v>
       </c>
       <c r="K35" s="5">
-        <v>0.33111468165473068</v>
+        <v>0.44193876092555606</v>
       </c>
       <c r="L35" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="N35" s="5">
         <v>0.70985736149037348</v>
@@ -24476,22 +24476,22 @@
         <v>44485</v>
       </c>
       <c r="F36" s="5">
-        <v>0.597097222010602</v>
+        <v>0.180899718201528</v>
       </c>
       <c r="G36" s="5">
-        <v>0.21698587777573469</v>
+        <v>0.35734753457032803</v>
       </c>
       <c r="H36" s="5">
-        <v>0.17718805657405112</v>
+        <v>0.42650275054141568</v>
       </c>
       <c r="J36" s="5">
-        <v>0.57334685554505349</v>
+        <v>0.17962564407093165</v>
       </c>
       <c r="K36" s="5">
-        <v>0.42211011863028364</v>
+        <v>0.82030589385705877</v>
       </c>
       <c r="L36" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="N36" s="5">
         <v>0.597097222010602</v>
@@ -24526,19 +24526,19 @@
         <v>44485</v>
       </c>
       <c r="F37" s="5">
-        <v>0.25674870827216073</v>
+        <v>0.36358861618702648</v>
       </c>
       <c r="G37" s="5">
-        <v>0.43628744610012221</v>
+        <v>0.33188648530299258</v>
       </c>
       <c r="H37" s="5">
-        <v>0.29529274359600216</v>
+        <v>0.28828934380803006</v>
       </c>
       <c r="J37" s="5">
-        <v>0.1036929140109325</v>
+        <v>0.26078768121650514</v>
       </c>
       <c r="K37" s="5">
-        <v>0.8963025152043731</v>
+        <v>0.73913007201895808</v>
       </c>
       <c r="L37" t="s">
         <v>20</v>
@@ -24576,22 +24576,22 @@
         <v>44485</v>
       </c>
       <c r="F38" s="5">
-        <v>0.59094999363013201</v>
+        <v>0.17933090092294224</v>
       </c>
       <c r="G38" s="5">
-        <v>0.23842874505931469</v>
+        <v>0.2968689668386193</v>
       </c>
       <c r="H38" s="5">
-        <v>0.16411303950591211</v>
+        <v>0.47179920396252384</v>
       </c>
       <c r="J38" s="5">
-        <v>0.4564614589812333</v>
+        <v>0.28850550356414023</v>
       </c>
       <c r="K38" s="5">
-        <v>0.54155466923713813</v>
+        <v>0.71114992702035507</v>
       </c>
       <c r="L38" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="N38" s="5">
         <v>0.59094999363013201</v>
@@ -24626,19 +24626,19 @@
         <v>44485</v>
       </c>
       <c r="F39" s="5">
-        <v>0.47947325538542135</v>
+        <v>0.5922557974795094</v>
       </c>
       <c r="G39" s="5">
-        <v>0.25609121174451466</v>
+        <v>0.23783904887255844</v>
       </c>
       <c r="H39" s="5">
-        <v>0.24955296548034922</v>
+        <v>0.16343614139259144</v>
       </c>
       <c r="J39" s="5">
-        <v>0.48415081659161024</v>
+        <v>0.45767462390861419</v>
       </c>
       <c r="K39" s="5">
-        <v>0.51464231343474309</v>
+        <v>0.5403079766595198</v>
       </c>
       <c r="L39" t="s">
         <v>16</v>
@@ -24676,22 +24676,22 @@
         <v>44485</v>
       </c>
       <c r="F40" s="5">
-        <v>0.37514169598477692</v>
+        <v>0.23249755694899998</v>
       </c>
       <c r="G40" s="5">
-        <v>0.30711163410783093</v>
+        <v>0.25953246676842873</v>
       </c>
       <c r="H40" s="5">
-        <v>0.29865817384007715</v>
+        <v>0.45698717283289603</v>
       </c>
       <c r="J40" s="5">
-        <v>0.3260668431028188</v>
+        <v>0.44138892485655834</v>
       </c>
       <c r="K40" s="5">
-        <v>0.67375320240234893</v>
+        <v>0.55758088757986501</v>
       </c>
       <c r="L40" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="N40" s="5">
         <v>0.37514169598477692</v>
@@ -24726,19 +24726,19 @@
         <v>44485</v>
       </c>
       <c r="F41" s="5">
-        <v>0.54945290511105438</v>
+        <v>0.48368680418583565</v>
       </c>
       <c r="G41" s="5">
-        <v>0.28853946991112595</v>
+        <v>0.31945993869034611</v>
       </c>
       <c r="H41" s="5">
-        <v>0.15742423195697008</v>
+        <v>0.19046219480991458</v>
       </c>
       <c r="J41" s="5">
-        <v>0.29478418590827227</v>
+        <v>0.25210861408224461</v>
       </c>
       <c r="K41" s="5">
-        <v>0.70477102349542087</v>
+        <v>0.74771242135076277</v>
       </c>
       <c r="L41" t="s">
         <v>20</v>
@@ -24776,19 +24776,19 @@
         <v>44485</v>
       </c>
       <c r="F42" s="5">
-        <v>0.41528520841650879</v>
+        <v>0.49152431488838533</v>
       </c>
       <c r="G42" s="5">
-        <v>0.27369873242541498</v>
+        <v>0.29535328792653032</v>
       </c>
       <c r="H42" s="5">
-        <v>0.29129441153342933</v>
+        <v>0.20467818396974655</v>
       </c>
       <c r="J42" s="5">
-        <v>0.43599628570633675</v>
+        <v>0.31793468987526158</v>
       </c>
       <c r="K42" s="5">
-        <v>0.56340958460069934</v>
+        <v>0.68171994062356867</v>
       </c>
       <c r="L42" t="s">
         <v>20</v>
@@ -24826,22 +24826,22 @@
         <v>44485</v>
       </c>
       <c r="F43" s="5">
-        <v>0.19973619134320289</v>
+        <v>0.37921784384371032</v>
       </c>
       <c r="G43" s="5">
-        <v>0.20137762698076006</v>
+        <v>0.26317408142872967</v>
       </c>
       <c r="H43" s="5">
-        <v>0.53242125043144195</v>
+        <v>0.33162657294140252</v>
       </c>
       <c r="J43" s="5">
-        <v>0.64727253314136968</v>
+        <v>0.48661946881213658</v>
       </c>
       <c r="K43" s="5">
-        <v>0.34536029625672771</v>
+        <v>0.51252581854064827</v>
       </c>
       <c r="L43" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="N43" s="5">
         <v>0.19973619134320289</v>
@@ -24876,22 +24876,22 @@
         <v>44485</v>
       </c>
       <c r="F44" s="5">
-        <v>0.50562091831823075</v>
+        <v>0.25139771292722496</v>
       </c>
       <c r="G44" s="5">
-        <v>0.23714990043760958</v>
+        <v>0.20242465400460857</v>
       </c>
       <c r="H44" s="5">
-        <v>0.24262964772686552</v>
+        <v>0.49285635873564893</v>
       </c>
       <c r="J44" s="5">
-        <v>0.56274749272451452</v>
+        <v>0.70982049901400845</v>
       </c>
       <c r="K44" s="5">
-        <v>0.43474088546994316</v>
+        <v>0.2811542194696201</v>
       </c>
       <c r="L44" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="N44" s="5">
         <v>0.50562091831823075</v>
@@ -24926,19 +24926,19 @@
         <v>44485</v>
       </c>
       <c r="F45" s="5">
-        <v>0.58368671474115774</v>
+        <v>0.72004133121976621</v>
       </c>
       <c r="G45" s="5">
-        <v>0.25232243854236541</v>
+        <v>0.1797848575310782</v>
       </c>
       <c r="H45" s="5">
-        <v>0.15841354858484905</v>
+        <v>9.5537682769767387E-2</v>
       </c>
       <c r="J45" s="5">
-        <v>0.3979045013918836</v>
+        <v>0.55233355789060212</v>
       </c>
       <c r="K45" s="5">
-        <v>0.60084008561544522</v>
+        <v>0.43942465872205194</v>
       </c>
       <c r="L45" t="s">
         <v>16</v>
@@ -24976,22 +24976,22 @@
         <v>44485</v>
       </c>
       <c r="F46" s="5">
-        <v>0.49986905429082451</v>
+        <v>0.16571633006510086</v>
       </c>
       <c r="G46" s="5">
-        <v>0.32880795012783937</v>
+        <v>0.1912674916573491</v>
       </c>
       <c r="H46" s="5">
-        <v>0.16693134858999045</v>
+        <v>0.56513554410194777</v>
       </c>
       <c r="J46" s="5">
-        <v>0.22007330088271182</v>
+        <v>0.63504359678224698</v>
       </c>
       <c r="K46" s="5">
-        <v>0.77977639520776643</v>
+        <v>0.3563668886850857</v>
       </c>
       <c r="L46" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="N46" s="5">
         <v>0.49986905429082451</v>
@@ -25026,22 +25026,22 @@
         <v>44485</v>
       </c>
       <c r="F47" s="5">
-        <v>0.41868003522171121</v>
+        <v>0.6519391116776424</v>
       </c>
       <c r="G47" s="5">
-        <v>0.32097785347306496</v>
+        <v>0.20508648742208455</v>
       </c>
       <c r="H47" s="5">
-        <v>0.24833378897493374</v>
+        <v>0.13714435235838479</v>
       </c>
       <c r="J47" s="5">
-        <v>0.27673274702026524</v>
+        <v>0.54810431459895093</v>
       </c>
       <c r="K47" s="5">
-        <v>0.72313219574619236</v>
+        <v>0.44657208332498555</v>
       </c>
       <c r="L47" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="N47" s="5">
         <v>0.41868003522171121</v>
@@ -25076,22 +25076,22 @@
         <v>44485</v>
       </c>
       <c r="F48" s="5">
-        <v>0.39597651017013019</v>
+        <v>0.16042450016862148</v>
       </c>
       <c r="G48" s="5">
-        <v>0.26934167208308635</v>
+        <v>0.23750898314664148</v>
       </c>
       <c r="H48" s="5">
-        <v>0.31185500733771926</v>
+        <v>0.5292706642204239</v>
       </c>
       <c r="J48" s="5">
-        <v>0.45845265121862316</v>
+        <v>0.43654699215627984</v>
       </c>
       <c r="K48" s="5">
-        <v>0.54086499728352377</v>
+        <v>0.56161430836285742</v>
       </c>
       <c r="L48" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="N48" s="5">
         <v>0.39597651017013019</v>
@@ -25126,22 +25126,22 @@
         <v>44485</v>
       </c>
       <c r="F49" s="5">
-        <v>0.11175413997466027</v>
+        <v>0.44019989572300883</v>
       </c>
       <c r="G49" s="5">
-        <v>0.19168776450624145</v>
+        <v>0.26563798515673792</v>
       </c>
       <c r="H49" s="5">
-        <v>0.59718506650888281</v>
+        <v>0.27620827659332381</v>
       </c>
       <c r="J49" s="5">
-        <v>0.51286292918489607</v>
+        <v>0.46148930667847465</v>
       </c>
       <c r="K49" s="5">
-        <v>0.48175438131556347</v>
+        <v>0.53768918883079442</v>
       </c>
       <c r="L49" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="N49" s="5">
         <v>0.11175413997466027</v>
@@ -25176,22 +25176,22 @@
         <v>44485</v>
       </c>
       <c r="F50" s="5">
-        <v>0.36495411134695899</v>
+        <v>0.56194171980187246</v>
       </c>
       <c r="G50" s="5">
-        <v>0.38939053616676628</v>
+        <v>0.21346925417069054</v>
       </c>
       <c r="H50" s="5">
-        <v>0.237448620720044</v>
+        <v>0.21203735449699207</v>
       </c>
       <c r="J50" s="5">
-        <v>0.15326284565651999</v>
+        <v>0.64718959673274445</v>
       </c>
       <c r="K50" s="5">
-        <v>0.84671834762027298</v>
+        <v>0.34654072308701322</v>
       </c>
       <c r="L50" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="N50" s="5">
         <v>0.36495411134695899</v>
@@ -25226,19 +25226,19 @@
         <v>44485</v>
       </c>
       <c r="F51" s="5">
-        <v>0.32346010682294418</v>
+        <v>0.39618605930387563</v>
       </c>
       <c r="G51" s="5">
-        <v>0.32284269395866549</v>
+        <v>0.30727619667718054</v>
       </c>
       <c r="H51" s="5">
-        <v>0.33095341379286847</v>
+        <v>0.27998360664834665</v>
       </c>
       <c r="J51" s="5">
-        <v>0.28402112844236221</v>
+        <v>0.32189053050410804</v>
       </c>
       <c r="K51" s="5">
-        <v>0.71587275290490049</v>
+        <v>0.67792221605889658</v>
       </c>
       <c r="L51" t="s">
         <v>20</v>
@@ -25276,22 +25276,22 @@
         <v>44485</v>
       </c>
       <c r="F52" s="5">
-        <v>0.80222585755090503</v>
+        <v>0.53295442685488459</v>
       </c>
       <c r="G52" s="5">
-        <v>0.1291158768235339</v>
+        <v>0.31588291026865595</v>
       </c>
       <c r="H52" s="5">
-        <v>5.3926498279988473E-2</v>
+        <v>0.14775494109398282</v>
       </c>
       <c r="J52" s="5">
-        <v>0.65891323917873768</v>
+        <v>0.22991819951484208</v>
       </c>
       <c r="K52" s="5">
-        <v>0.31220962312047645</v>
+        <v>0.76986243917959019</v>
       </c>
       <c r="L52" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="N52" s="5">
         <v>0.80222585755090503</v>
@@ -25326,22 +25326,22 @@
         <v>44485</v>
       </c>
       <c r="F53" s="5">
-        <v>9.5284142231627771E-3</v>
+        <v>0.21986474253086621</v>
       </c>
       <c r="G53" s="5">
-        <v>5.8317083096674889E-2</v>
+        <v>0.28113948799852606</v>
       </c>
       <c r="H53" s="5">
-        <v>0.70432111015063403</v>
+        <v>0.45049625552874401</v>
       </c>
       <c r="J53" s="5">
-        <v>0.61203541644127513</v>
+        <v>0.36046780665628603</v>
       </c>
       <c r="K53" s="5">
-        <v>0.34419131956309879</v>
+        <v>0.63901412648506573</v>
       </c>
       <c r="L53" t="s">
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="N53" s="5">
         <v>9.5284142231627771E-3</v>
@@ -25376,22 +25376,22 @@
         <v>44485</v>
       </c>
       <c r="F54" s="5">
-        <v>4.2442415233864675E-2</v>
+        <v>0.43789204639958296</v>
       </c>
       <c r="G54" s="5">
-        <v>0.19066325081530522</v>
+        <v>0.25201156753499221</v>
       </c>
       <c r="H54" s="5">
-        <v>0.63671340254507147</v>
+        <v>0.28998146214264359</v>
       </c>
       <c r="J54" s="5">
-        <v>0.33431088376488172</v>
+        <v>0.52596452921480408</v>
       </c>
       <c r="K54" s="5">
-        <v>0.66302746921533862</v>
+        <v>0.47265675257619411</v>
       </c>
       <c r="L54" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="N54" s="5">
         <v>4.2442415233864675E-2</v>
@@ -25426,22 +25426,22 @@
         <v>44485</v>
       </c>
       <c r="F55" s="5">
-        <v>0.66019045661124642</v>
+        <v>0.48292264054694906</v>
       </c>
       <c r="G55" s="5">
-        <v>0.2811080645850258</v>
+        <v>0.29742586164434437</v>
       </c>
       <c r="H55" s="5">
-        <v>5.8248191850493618E-2</v>
+        <v>0.21068561689608528</v>
       </c>
       <c r="J55" s="5">
-        <v>0.19942195737003751</v>
+        <v>0.3166449622347568</v>
       </c>
       <c r="K55" s="5">
-        <v>0.80013450036827538</v>
+        <v>0.6830352935088978</v>
       </c>
       <c r="L55" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="N55" s="5">
         <v>0.66019045661124642</v>
@@ -25476,22 +25476,22 @@
         <v>44485</v>
       </c>
       <c r="F56" s="5">
-        <v>0.47761383062683871</v>
+        <v>0.25334190269234869</v>
       </c>
       <c r="G56" s="5">
-        <v>0.34993556340002935</v>
+        <v>0.34904048668837678</v>
       </c>
       <c r="H56" s="5">
-        <v>0.16837495669053862</v>
+        <v>0.37083163331149377</v>
       </c>
       <c r="J56" s="5">
-        <v>0.18693527234394089</v>
+        <v>0.21645566024426774</v>
       </c>
       <c r="K56" s="5">
-        <v>0.81297819640795232</v>
+        <v>0.78348553713148239</v>
       </c>
       <c r="L56" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="N56" s="5">
         <v>0.47761383062683871</v>
@@ -25526,22 +25526,22 @@
         <v>44485</v>
       </c>
       <c r="F57" s="5">
-        <v>0.72048589888253101</v>
+        <v>0.45976380653038063</v>
       </c>
       <c r="G57" s="5">
-        <v>0.1963381822443068</v>
+        <v>0.26746839851778176</v>
       </c>
       <c r="H57" s="5">
-        <v>8.0824254959638825E-2</v>
+        <v>0.25730923334265238</v>
       </c>
       <c r="J57" s="5">
-        <v>0.43270905339621379</v>
+        <v>0.44396969300425088</v>
       </c>
       <c r="K57" s="5">
-        <v>0.5634221911020254</v>
+        <v>0.55524259679896448</v>
       </c>
       <c r="L57" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="N57" s="5">
         <v>0.72048589888253101</v>
@@ -25576,22 +25576,22 @@
         <v>44485</v>
       </c>
       <c r="F58" s="5">
-        <v>0.27157164490315261</v>
+        <v>0.27218101923113036</v>
       </c>
       <c r="G58" s="5">
-        <v>0.30084314920594163</v>
+        <v>0.24342402440769534</v>
       </c>
       <c r="H58" s="5">
-        <v>0.39273918499380239</v>
+        <v>0.438565034438753</v>
       </c>
       <c r="J58" s="5">
-        <v>0.33185619144101475</v>
+        <v>0.53737139682615864</v>
       </c>
       <c r="K58" s="5">
-        <v>0.66789744540505147</v>
+        <v>0.46078260074044708</v>
       </c>
       <c r="L58" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="N58" s="5">
         <v>0.27157164490315261</v>
@@ -25626,22 +25626,22 @@
         <v>44485</v>
       </c>
       <c r="F59" s="5">
-        <v>0.16001914177398988</v>
+        <v>0.32094732034162171</v>
       </c>
       <c r="G59" s="5">
-        <v>0.34751429258476657</v>
+        <v>0.30271050309511416</v>
       </c>
       <c r="H59" s="5">
-        <v>0.45143853448870624</v>
+        <v>0.34928563614186808</v>
       </c>
       <c r="J59" s="5">
-        <v>0.18430246225773303</v>
+        <v>0.33907819493092789</v>
       </c>
       <c r="K59" s="5">
-        <v>0.81560120908690648</v>
+        <v>0.66071468619599971</v>
       </c>
       <c r="L59" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="N59" s="5">
         <v>0.16001914177398988</v>
@@ -25676,19 +25676,19 @@
         <v>44485</v>
       </c>
       <c r="F60" s="5">
-        <v>0.52162739065969033</v>
+        <v>0.227186236472049</v>
       </c>
       <c r="G60" s="5">
-        <v>0.29374814137465743</v>
+        <v>0.28126992838433212</v>
       </c>
       <c r="H60" s="5">
-        <v>0.17851250537763105</v>
+        <v>0.44445859980259528</v>
       </c>
       <c r="J60" s="5">
-        <v>0.30143336022508843</v>
+        <v>0.36535491874418086</v>
       </c>
       <c r="K60" s="5">
-        <v>0.69818748225878646</v>
+        <v>0.63413410565098294</v>
       </c>
       <c r="L60" t="s">
         <v>20</v>
@@ -25726,22 +25726,22 @@
         <v>44485</v>
       </c>
       <c r="F61" s="5">
-        <v>0.27267836561724784</v>
+        <v>0.49306727229485847</v>
       </c>
       <c r="G61" s="5">
-        <v>0.72732158454769191</v>
+        <v>0.25139684164420123</v>
       </c>
       <c r="H61" s="5">
-        <v>0</v>
+        <v>0.24147135271612447</v>
       </c>
       <c r="J61" s="5">
-        <v>4.2446583658954651E-3</v>
+        <v>0.49746054666078304</v>
       </c>
       <c r="K61" s="5">
-        <v>0.99575529179904421</v>
+        <v>0.50109742722406092</v>
       </c>
       <c r="L61" t="s">
-        <v>133</v>
+        <v>16</v>
       </c>
       <c r="N61" s="5">
         <v>0.27267836561724784</v>
@@ -25776,22 +25776,22 @@
         <v>44485</v>
       </c>
       <c r="F62" s="5">
-        <v>0.83296499391601198</v>
+        <v>0.40176332981279661</v>
       </c>
       <c r="G62" s="5">
-        <v>0.132220348332905</v>
+        <v>0.28131312270587444</v>
       </c>
       <c r="H62" s="5">
-        <v>2.8962402241575331E-2</v>
+        <v>0.29674729187762772</v>
       </c>
       <c r="J62" s="5">
-        <v>0.46759010489246527</v>
+        <v>0.40927145579526325</v>
       </c>
       <c r="K62" s="5">
-        <v>0.5224934714040087</v>
+        <v>0.59028350111627037</v>
       </c>
       <c r="L62" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="N62" s="5">
         <v>0.83296499391601198</v>
@@ -25826,19 +25826,19 @@
         <v>44485</v>
       </c>
       <c r="F63" s="5">
-        <v>0.33205857842809744</v>
+        <v>0.37923946433867717</v>
       </c>
       <c r="G63" s="5">
-        <v>0.33669432180849307</v>
+        <v>0.29403133872633819</v>
       </c>
       <c r="H63" s="5">
-        <v>0.31215661454888338</v>
+        <v>0.30586958254564717</v>
       </c>
       <c r="J63" s="5">
-        <v>0.25132864405650768</v>
+        <v>0.36733918097014734</v>
       </c>
       <c r="K63" s="5">
-        <v>0.7486029506942351</v>
+        <v>0.6323822697694782</v>
       </c>
       <c r="L63" t="s">
         <v>20</v>
@@ -25876,22 +25876,22 @@
         <v>44485</v>
       </c>
       <c r="F64" s="5">
-        <v>0.30913684568345773</v>
+        <v>0.13735696385125842</v>
       </c>
       <c r="G64" s="5">
-        <v>0.21440845156595192</v>
+        <v>0.31131446185315875</v>
       </c>
       <c r="H64" s="5">
-        <v>0.43500964819340587</v>
+        <v>0.49569745507347246</v>
       </c>
       <c r="J64" s="5">
-        <v>0.70075298094687855</v>
+        <v>0.22702495516779764</v>
       </c>
       <c r="K64" s="5">
-        <v>0.29283862533050059</v>
+        <v>0.77272729297272003</v>
       </c>
       <c r="L64" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="N64" s="5">
         <v>0.30913684568345773</v>
@@ -25926,22 +25926,22 @@
         <v>44485</v>
       </c>
       <c r="F65" s="5">
-        <v>0.26865106689448048</v>
+        <v>0.59729615957564619</v>
       </c>
       <c r="G65" s="5">
-        <v>0.2623479096523938</v>
+        <v>0.20258958789887371</v>
       </c>
       <c r="H65" s="5">
-        <v>0.42551600459379313</v>
+        <v>0.18864934254183804</v>
       </c>
       <c r="J65" s="5">
-        <v>0.45757868127735918</v>
+        <v>0.670327890173677</v>
       </c>
       <c r="K65" s="5">
-        <v>0.5415000441244765</v>
+        <v>0.32069598455960974</v>
       </c>
       <c r="L65" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="N65" s="5">
         <v>0.26865106689448048</v>
@@ -25976,22 +25976,22 @@
         <v>44485</v>
       </c>
       <c r="F66" s="5">
-        <v>0.24496983079188683</v>
+        <v>0.53882625742011947</v>
       </c>
       <c r="G66" s="5">
-        <v>0.23682350976848307</v>
+        <v>0.27151980843229451</v>
       </c>
       <c r="H66" s="5">
-        <v>0.46601493662213289</v>
+        <v>0.18253375444172118</v>
       </c>
       <c r="J66" s="5">
-        <v>0.54305610726215858</v>
+        <v>0.36635784564398682</v>
       </c>
       <c r="K66" s="5">
-        <v>0.45464220818771017</v>
+        <v>0.63291608438653413</v>
       </c>
       <c r="L66" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="N66" s="5">
         <v>0.24496983079188683</v>
@@ -26025,23 +26025,23 @@
       <c r="D67" s="4">
         <v>44485</v>
       </c>
-      <c r="F67" s="5">
-        <v>0.75983746124095797</v>
-      </c>
-      <c r="G67" s="5">
-        <v>0.1997630244591222</v>
-      </c>
-      <c r="H67" s="5">
-        <v>3.918452626923883E-2</v>
-      </c>
-      <c r="J67" s="5">
-        <v>0.30880633862547724</v>
-      </c>
-      <c r="K67" s="5">
-        <v>0.6890340463021164</v>
-      </c>
-      <c r="L67" t="s">
-        <v>37</v>
+      <c r="F67" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G67" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H67" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J67" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K67" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L67" t="e">
+        <v>#N/A</v>
       </c>
       <c r="N67" s="5">
         <v>0.75983746124095797</v>
@@ -26076,22 +26076,22 @@
         <v>44485</v>
       </c>
       <c r="F68" s="5">
-        <v>9.6575905918552848E-2</v>
+        <v>0.27048959798326466</v>
       </c>
       <c r="G68" s="5">
-        <v>0.23811259859447609</v>
+        <v>0.24628171071845001</v>
       </c>
       <c r="H68" s="5">
-        <v>0.57442880631193005</v>
+        <v>0.43746009377786971</v>
       </c>
       <c r="J68" s="5">
-        <v>0.33244028667158471</v>
+        <v>0.52380856345063509</v>
       </c>
       <c r="K68" s="5">
-        <v>0.66620521969788504</v>
+        <v>0.47453512484214055</v>
       </c>
       <c r="L68" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="N68" s="5">
         <v>9.6575905918552848E-2</v>
@@ -26126,22 +26126,22 @@
         <v>44485</v>
       </c>
       <c r="F69" s="5">
-        <v>9.7252003546893548E-2</v>
+        <v>0.28645345858651533</v>
       </c>
       <c r="G69" s="5">
-        <v>0.41962085348964651</v>
+        <v>0.30783401715338393</v>
       </c>
       <c r="H69" s="5">
-        <v>0.45083322729012337</v>
+        <v>0.37470429699361146</v>
       </c>
       <c r="J69" s="5">
-        <v>8.8862231479739706E-2</v>
+        <v>0.31727556444931282</v>
       </c>
       <c r="K69" s="5">
-        <v>0.91111356883206618</v>
+        <v>0.68253673877808274</v>
       </c>
       <c r="L69" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="N69" s="5">
         <v>9.7252003546893548E-2</v>
@@ -26175,23 +26175,23 @@
       <c r="D70" s="4">
         <v>44485</v>
       </c>
-      <c r="F70" s="5">
-        <v>0.51334812868651358</v>
-      </c>
-      <c r="G70" s="5">
-        <v>0.31773727053192524</v>
-      </c>
-      <c r="H70" s="5">
-        <v>0.16446290298219093</v>
-      </c>
-      <c r="J70" s="5">
-        <v>0.2386077974877073</v>
-      </c>
-      <c r="K70" s="5">
-        <v>0.7611899783888374</v>
-      </c>
-      <c r="L70" t="s">
-        <v>20</v>
+      <c r="F70" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G70" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H70" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J70" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K70" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L70" t="e">
+        <v>#N/A</v>
       </c>
       <c r="N70" s="5">
         <v>0.51334812868651358</v>
@@ -26226,22 +26226,22 @@
         <v>44485</v>
       </c>
       <c r="F71" s="5">
-        <v>0.50685445008626773</v>
+        <v>0.32941659171117915</v>
       </c>
       <c r="G71" s="5">
-        <v>0.25769198162525392</v>
+        <v>0.29765918564415156</v>
       </c>
       <c r="H71" s="5">
-        <v>0.22363816391352173</v>
+        <v>0.34606436246698757</v>
       </c>
       <c r="J71" s="5">
-        <v>0.45582733506206413</v>
+        <v>0.35565093046614665</v>
       </c>
       <c r="K71" s="5">
-        <v>0.54302608808968589</v>
+        <v>0.6441052603582359</v>
       </c>
       <c r="L71" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="N71" s="5">
         <v>0.50685445008626773</v>
@@ -26276,19 +26276,19 @@
         <v>44485</v>
       </c>
       <c r="F72" s="5">
-        <v>0.1715151700811883</v>
+        <v>0.23399741989268308</v>
       </c>
       <c r="G72" s="5">
-        <v>0.30615594098507787</v>
+        <v>0.3174870928826346</v>
       </c>
       <c r="H72" s="5">
-        <v>0.47155665950264836</v>
+        <v>0.41160172898375402</v>
       </c>
       <c r="J72" s="5">
-        <v>0.26243958365234499</v>
+        <v>0.27422005691477419</v>
       </c>
       <c r="K72" s="5">
-        <v>0.73728946403694284</v>
+        <v>0.72561466546995368</v>
       </c>
       <c r="L72" t="s">
         <v>20</v>
@@ -26326,22 +26326,22 @@
         <v>44485</v>
       </c>
       <c r="F73" s="5">
-        <v>2.1693892745655034E-2</v>
+        <v>0.25814924135459505</v>
       </c>
       <c r="G73" s="5">
-        <v>8.0497336354659624E-2</v>
+        <v>0.24904348020217812</v>
       </c>
       <c r="H73" s="5">
-        <v>0.70308687170226447</v>
+        <v>0.44505514251407619</v>
       </c>
       <c r="J73" s="5">
-        <v>0.6156144402144591</v>
+        <v>0.50293548446629488</v>
       </c>
       <c r="K73" s="5">
-        <v>0.35021241019252158</v>
+        <v>0.49557450946592374</v>
       </c>
       <c r="L73" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="N73" s="5">
         <v>2.1693892745655034E-2</v>
@@ -26375,23 +26375,23 @@
       <c r="D74" s="4">
         <v>44485</v>
       </c>
-      <c r="F74" s="5">
-        <v>0.46025540972949996</v>
-      </c>
-      <c r="G74" s="5">
-        <v>0.17707692264231376</v>
-      </c>
-      <c r="H74" s="5">
-        <v>0.30802768171282829</v>
-      </c>
-      <c r="J74" s="5">
-        <v>0.86738225282841097</v>
-      </c>
-      <c r="K74" s="5">
-        <v>7.8948413073571491E-2</v>
-      </c>
-      <c r="L74" t="s">
-        <v>410</v>
+      <c r="F74" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G74" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H74" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J74" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K74" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L74" t="e">
+        <v>#N/A</v>
       </c>
       <c r="N74" s="5">
         <v>0.46025540972949996</v>
@@ -26425,23 +26425,23 @@
       <c r="D75" s="4">
         <v>44485</v>
       </c>
-      <c r="F75" s="5">
-        <v>0.43482344776683607</v>
-      </c>
-      <c r="G75" s="5">
-        <v>0.39226703114172262</v>
-      </c>
-      <c r="H75" s="5">
-        <v>0.16946871250850135</v>
-      </c>
-      <c r="J75" s="5">
-        <v>0.13425284010704561</v>
-      </c>
-      <c r="K75" s="5">
-        <v>0.86571796612002672</v>
-      </c>
-      <c r="L75" t="s">
-        <v>17</v>
+      <c r="F75" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G75" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H75" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J75" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K75" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L75" t="e">
+        <v>#N/A</v>
       </c>
       <c r="N75" s="5">
         <v>0.43482344776683607</v>
@@ -26476,22 +26476,22 @@
         <v>44485</v>
       </c>
       <c r="F76" s="5">
-        <v>0.75059086920621665</v>
+        <v>0.79460958271504689</v>
       </c>
       <c r="G76" s="5">
-        <v>0.12772476802508687</v>
+        <v>0.15277890053764362</v>
       </c>
       <c r="H76" s="5">
-        <v>6.5561548807454406E-2</v>
+        <v>4.8437446485384221E-2</v>
       </c>
       <c r="J76" s="5">
-        <v>0.77847957896432385</v>
+        <v>0.48441187032453048</v>
       </c>
       <c r="K76" s="5">
-        <v>0.13387147640974739</v>
+        <v>0.50702965621418117</v>
       </c>
       <c r="L76" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="N76" s="5">
         <v>0.75059086920621665</v>
@@ -26526,22 +26526,22 @@
         <v>44485</v>
       </c>
       <c r="F77" s="5">
-        <v>0.87239989377994542</v>
+        <v>0.77409317078851547</v>
       </c>
       <c r="G77" s="5">
-        <v>6.7929649085793159E-2</v>
+        <v>0.13989694736721328</v>
       </c>
       <c r="H77" s="5">
-        <v>1.1429582550092273E-2</v>
+        <v>7.0482766610872563E-2</v>
       </c>
       <c r="J77" s="5">
-        <v>0.66134103609771711</v>
+        <v>0.69106422295235981</v>
       </c>
       <c r="K77" s="5">
-        <v>0.27436410847454323</v>
+        <v>0.27845059777197806</v>
       </c>
       <c r="L77" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="N77" s="5">
         <v>0.87239989377994542</v>
@@ -26576,22 +26576,22 @@
         <v>44485</v>
       </c>
       <c r="F78" s="5">
-        <v>0.80564221545639803</v>
+        <v>0.24006126608918285</v>
       </c>
       <c r="G78" s="5">
-        <v>0.19279072592719615</v>
+        <v>0.38537274851743381</v>
       </c>
       <c r="H78" s="5">
-        <v>0</v>
+        <v>0.35332630109444857</v>
       </c>
       <c r="J78" s="5">
-        <v>0.22706666056913521</v>
+        <v>0.15757389421596793</v>
       </c>
       <c r="K78" s="5">
-        <v>0.77136628081445902</v>
+        <v>0.84240419261557542</v>
       </c>
       <c r="L78" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="N78" s="5">
         <v>0.80564221545639803</v>
@@ -26626,19 +26626,19 @@
         <v>44485</v>
       </c>
       <c r="F79" s="5">
-        <v>0.38614533661305661</v>
+        <v>0.50968633776857752</v>
       </c>
       <c r="G79" s="5">
-        <v>0.29246658558383859</v>
+        <v>0.28893782920464606</v>
       </c>
       <c r="H79" s="5">
-        <v>0.30112902075578823</v>
+        <v>0.19376225170317529</v>
       </c>
       <c r="J79" s="5">
-        <v>0.37171286051976132</v>
+        <v>0.32669631777119229</v>
       </c>
       <c r="K79" s="5">
-        <v>0.62799069817460595</v>
+        <v>0.67287658838960096</v>
       </c>
       <c r="L79" t="s">
         <v>20</v>
@@ -26676,22 +26676,22 @@
         <v>44485</v>
       </c>
       <c r="F80" s="5">
-        <v>0.60588893540388444</v>
+        <v>8.0442106880731015E-2</v>
       </c>
       <c r="G80" s="5">
-        <v>0.2689292789527184</v>
+        <v>0.13521864550972307</v>
       </c>
       <c r="H80" s="5">
-        <v>0.12248399944629908</v>
+        <v>0.66080246855515379</v>
       </c>
       <c r="J80" s="5">
-        <v>0.30175474276829595</v>
+        <v>0.66409295168808735</v>
       </c>
       <c r="K80" s="5">
-        <v>0.69752894962737699</v>
+        <v>0.31328180855449494</v>
       </c>
       <c r="L80" t="s">
-        <v>17</v>
+        <v>72</v>
       </c>
       <c r="N80" s="5">
         <v>0.60588893540388444</v>
@@ -26726,22 +26726,22 @@
         <v>44485</v>
       </c>
       <c r="F81" s="5">
-        <v>0.56793306926136566</v>
+        <v>0.51762004182676158</v>
       </c>
       <c r="G81" s="5">
-        <v>0.37072221135640737</v>
+        <v>0.31030910154717362</v>
       </c>
       <c r="H81" s="5">
-        <v>6.1099476336124642E-2</v>
+        <v>0.16725900249843342</v>
       </c>
       <c r="J81" s="5">
-        <v>0.10941609093547787</v>
+        <v>0.25524827564558217</v>
       </c>
       <c r="K81" s="5">
-        <v>0.89050867505358322</v>
+        <v>0.74450696651417647</v>
       </c>
       <c r="L81" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="N81" s="5">
         <v>0.56793306926136566</v>
@@ -26776,22 +26776,22 @@
         <v>44485</v>
       </c>
       <c r="F82" s="5">
-        <v>0.49771999453612614</v>
+        <v>0.18192050944536853</v>
       </c>
       <c r="G82" s="5">
-        <v>0.21003186506019939</v>
+        <v>0.22428385970621434</v>
       </c>
       <c r="H82" s="5">
-        <v>0.27281740900332457</v>
+        <v>0.52434633621819637</v>
       </c>
       <c r="J82" s="5">
-        <v>0.72826512221442175</v>
+        <v>0.51858280729934514</v>
       </c>
       <c r="K82" s="5">
-        <v>0.26282339539818322</v>
+        <v>0.47839399053854914</v>
       </c>
       <c r="L82" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="N82" s="5">
         <v>0.49771999453612614</v>
@@ -26826,22 +26826,22 @@
         <v>44485</v>
       </c>
       <c r="F83" s="5">
-        <v>0.47681677818658064</v>
+        <v>0.6126694784818798</v>
       </c>
       <c r="G83" s="5">
-        <v>0.31326132084446595</v>
+        <v>0.31234717084496216</v>
       </c>
       <c r="H83" s="5">
-        <v>0.20230757650330572</v>
+        <v>7.4403916618711749E-2</v>
       </c>
       <c r="J83" s="5">
-        <v>0.27256704047986841</v>
+        <v>0.17488088876496419</v>
       </c>
       <c r="K83" s="5">
-        <v>0.72722793785190809</v>
+        <v>0.82487719758314249</v>
       </c>
       <c r="L83" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="N83" s="5">
         <v>0.47681677818658064</v>
@@ -26976,22 +26976,22 @@
         <v>44485</v>
       </c>
       <c r="F86" s="5">
-        <v>0</v>
+        <v>0.69880382183991407</v>
       </c>
       <c r="G86" s="5">
-        <v>0.22992548518672384</v>
+        <v>0.2035266279384802</v>
       </c>
       <c r="H86" s="5">
-        <v>0.64752249156971631</v>
+        <v>9.4904572792831945E-2</v>
       </c>
       <c r="J86" s="5">
-        <v>0.18283630320553446</v>
+        <v>0.4454881881749696</v>
       </c>
       <c r="K86" s="5">
-        <v>0.81633893888120379</v>
+        <v>0.5508456543753868</v>
       </c>
       <c r="L86" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="N86" s="5">
         <v>0</v>
@@ -27126,22 +27126,22 @@
         <v>44486</v>
       </c>
       <c r="F89" s="5">
-        <v>0.41599151399144796</v>
+        <v>0.64831701946333031</v>
       </c>
       <c r="G89" s="5">
-        <v>0.25948271695577835</v>
+        <v>0.19850096586515373</v>
       </c>
       <c r="H89" s="5">
-        <v>0.30277294847949549</v>
+        <v>0.14584255944095167</v>
       </c>
       <c r="J89" s="5">
-        <v>0.49757745338694637</v>
+        <v>0.60319498346408518</v>
       </c>
       <c r="K89" s="5">
-        <v>0.50141142828462948</v>
+        <v>0.38931700013696596</v>
       </c>
       <c r="L89" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="N89" s="5">
         <v>0.41599151399144796</v>
@@ -27176,22 +27176,22 @@
         <v>44486</v>
       </c>
       <c r="F90" s="5">
-        <v>0.651010488485257</v>
+        <v>0.41667702309301402</v>
       </c>
       <c r="G90" s="5">
-        <v>0.22297663519628555</v>
+        <v>0.33414961250549513</v>
       </c>
       <c r="H90" s="5">
-        <v>0.12228116855266737</v>
+        <v>0.23877541446174377</v>
       </c>
       <c r="J90" s="5">
-        <v>0.43797540213051167</v>
+        <v>0.24432751342288281</v>
       </c>
       <c r="K90" s="5">
-        <v>0.55944559206514943</v>
+        <v>0.75557818293832568</v>
       </c>
       <c r="L90" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="N90" s="5">
         <v>0.651010488485257</v>
@@ -27225,23 +27225,23 @@
       <c r="D91" s="4">
         <v>44486</v>
       </c>
-      <c r="F91" s="5">
-        <v>0.13516597650977666</v>
-      </c>
-      <c r="G91" s="5">
-        <v>0.22248125237043262</v>
-      </c>
-      <c r="H91" s="5">
-        <v>0.55843426067675672</v>
-      </c>
-      <c r="J91" s="5">
-        <v>0.44748761034557466</v>
-      </c>
-      <c r="K91" s="5">
-        <v>0.54995482677414942</v>
-      </c>
-      <c r="L91" t="s">
-        <v>28</v>
+      <c r="F91" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G91" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H91" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J91" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K91" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L91" t="e">
+        <v>#N/A</v>
       </c>
       <c r="N91" s="5">
         <v>0.13516597650977666</v>
@@ -27276,22 +27276,22 @@
         <v>44486</v>
       </c>
       <c r="F92" s="5">
-        <v>0.18410281553360799</v>
+        <v>0.60616327688609473</v>
       </c>
       <c r="G92" s="5">
-        <v>0.25542988422045254</v>
+        <v>0.21798869528920392</v>
       </c>
       <c r="H92" s="5">
-        <v>0.49802642628903387</v>
+        <v>0.16806271451586074</v>
       </c>
       <c r="J92" s="5">
-        <v>0.40715735070010967</v>
+        <v>0.5517628282216207</v>
       </c>
       <c r="K92" s="5">
-        <v>0.59170627962866584</v>
+        <v>0.44409225028091498</v>
       </c>
       <c r="L92" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="N92" s="5">
         <v>0.18410281553360799</v>
@@ -27325,23 +27325,23 @@
       <c r="D93" s="4">
         <v>44486</v>
       </c>
-      <c r="F93" s="5">
-        <v>0.66824338331787791</v>
-      </c>
-      <c r="G93" s="5">
-        <v>0.20211895632180518</v>
-      </c>
-      <c r="H93" s="5">
-        <v>0.12467130032021664</v>
-      </c>
-      <c r="J93" s="5">
-        <v>0.53098521691304446</v>
-      </c>
-      <c r="K93" s="5">
-        <v>0.46375705784725663</v>
-      </c>
-      <c r="L93" t="s">
-        <v>16</v>
+      <c r="F93" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G93" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H93" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J93" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K93" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L93" t="e">
+        <v>#N/A</v>
       </c>
       <c r="N93" s="5">
         <v>0.66824338331787791</v>
@@ -27375,23 +27375,23 @@
       <c r="D94" s="4">
         <v>44486</v>
       </c>
-      <c r="F94" s="5">
-        <v>0.18637696415881941</v>
-      </c>
-      <c r="G94" s="5">
-        <v>0.19105165735274982</v>
-      </c>
-      <c r="H94" s="5">
-        <v>0.55160203165406596</v>
-      </c>
-      <c r="J94" s="5">
-        <v>0.67384248044100792</v>
-      </c>
-      <c r="K94" s="5">
-        <v>0.31613279228535868</v>
-      </c>
-      <c r="L94" t="s">
-        <v>28</v>
+      <c r="F94" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G94" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H94" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J94" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K94" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L94" t="e">
+        <v>#N/A</v>
       </c>
       <c r="N94" s="5">
         <v>0.18637696415881941</v>
@@ -27426,22 +27426,22 @@
         <v>44486</v>
       </c>
       <c r="F95" s="5">
-        <v>0.12477723173823177</v>
+        <v>0.83278687433401821</v>
       </c>
       <c r="G95" s="5">
-        <v>0.2574312259551893</v>
+        <v>0.10393545183669353</v>
       </c>
       <c r="H95" s="5">
-        <v>0.54145500753495479</v>
+        <v>3.3441749709009455E-2</v>
       </c>
       <c r="J95" s="5">
-        <v>0.32664985590932372</v>
+        <v>0.68893578442547654</v>
       </c>
       <c r="K95" s="5">
-        <v>0.67241193890702222</v>
+        <v>0.26086631942396249</v>
       </c>
       <c r="L95" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="N95" s="5">
         <v>0.12477723173823177</v>
@@ -27476,22 +27476,22 @@
         <v>44486</v>
       </c>
       <c r="F96" s="5">
-        <v>0.44351781586497785</v>
+        <v>0.57688763830516454</v>
       </c>
       <c r="G96" s="5">
-        <v>0.38710992163322056</v>
+        <v>0.22968034003117271</v>
       </c>
       <c r="H96" s="5">
-        <v>0.16603807753041447</v>
+        <v>0.1846557280011959</v>
       </c>
       <c r="J96" s="5">
-        <v>0.13873697581866512</v>
+        <v>0.52566937182629614</v>
       </c>
       <c r="K96" s="5">
-        <v>0.86122896386660164</v>
+        <v>0.47141810023279546</v>
       </c>
       <c r="L96" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="N96" s="5">
         <v>0.44351781586497785</v>
@@ -27526,19 +27526,19 @@
         <v>44486</v>
       </c>
       <c r="F97" s="5">
-        <v>0.71935178063988225</v>
+        <v>0.49391278490819662</v>
       </c>
       <c r="G97" s="5">
-        <v>0.17476795939997827</v>
+        <v>0.23175598388790122</v>
       </c>
       <c r="H97" s="5">
-        <v>9.9910198394282751E-2</v>
+        <v>0.25786707070773118</v>
       </c>
       <c r="J97" s="5">
-        <v>0.59576122438545587</v>
+        <v>0.60251557719347792</v>
       </c>
       <c r="K97" s="5">
-        <v>0.39338403761988794</v>
+        <v>0.39429124873030524</v>
       </c>
       <c r="L97" t="s">
         <v>16</v>
@@ -27576,22 +27576,22 @@
         <v>44486</v>
       </c>
       <c r="F98" s="5">
-        <v>0.58293027039824319</v>
+        <v>0.27098993540373617</v>
       </c>
       <c r="G98" s="5">
-        <v>0.23275634344621188</v>
+        <v>0.23677029327715554</v>
       </c>
       <c r="H98" s="5">
-        <v>0.17645649689765106</v>
+        <v>0.44538816851171453</v>
       </c>
       <c r="J98" s="5">
-        <v>0.49926605082455122</v>
+        <v>0.5659893162958467</v>
       </c>
       <c r="K98" s="5">
-        <v>0.49820898384409573</v>
+        <v>0.43163144936540659</v>
       </c>
       <c r="L98" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="N98" s="5">
         <v>0.58293027039824319</v>
@@ -27626,22 +27626,22 @@
         <v>44486</v>
       </c>
       <c r="F99" s="5">
-        <v>0.63527490892179816</v>
+        <v>0.21928123007434813</v>
       </c>
       <c r="G99" s="5">
-        <v>0.19991696640943035</v>
+        <v>0.19947204063743795</v>
       </c>
       <c r="H99" s="5">
-        <v>0.15651476094105904</v>
+        <v>0.52009182224358119</v>
       </c>
       <c r="J99" s="5">
-        <v>0.62067722061258657</v>
+        <v>0.68469724796831322</v>
       </c>
       <c r="K99" s="5">
-        <v>0.37150943023516042</v>
+        <v>0.30651599190796797</v>
       </c>
       <c r="L99" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="N99" s="5">
         <v>0.63527490892179816</v>
@@ -27676,22 +27676,22 @@
         <v>44486</v>
       </c>
       <c r="F100" s="5">
-        <v>0.21513568647322512</v>
+        <v>0.31662987264187348</v>
       </c>
       <c r="G100" s="5">
-        <v>0.24704452276659628</v>
+        <v>0.29983243245603092</v>
       </c>
       <c r="H100" s="5">
-        <v>0.48065768124083763</v>
+        <v>0.35528714825317798</v>
       </c>
       <c r="J100" s="5">
-        <v>0.47118114885895385</v>
+        <v>0.34710361741275192</v>
       </c>
       <c r="K100" s="5">
-        <v>0.52727165297397316</v>
+        <v>0.65266644458519751</v>
       </c>
       <c r="L100" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="N100" s="5">
         <v>0.21513568647322512</v>
@@ -27726,22 +27726,22 @@
         <v>44486</v>
       </c>
       <c r="F101" s="5">
-        <v>0.27714349442046304</v>
+        <v>0.40677323074673943</v>
       </c>
       <c r="G101" s="5">
-        <v>0.33177500714250208</v>
+        <v>0.22222657745409569</v>
       </c>
       <c r="H101" s="5">
-        <v>0.36389802431608531</v>
+        <v>0.34396063437065771</v>
       </c>
       <c r="J101" s="5">
-        <v>0.2563508142637978</v>
+        <v>0.68919692741041338</v>
       </c>
       <c r="K101" s="5">
-        <v>0.74355945108090538</v>
+        <v>0.30575993242980781</v>
       </c>
       <c r="L101" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="N101" s="5">
         <v>0.27714349442046304</v>
@@ -27776,19 +27776,19 @@
         <v>44486</v>
       </c>
       <c r="F102" s="5">
-        <v>0.41528603610482689</v>
+        <v>0.35041457331550463</v>
       </c>
       <c r="G102" s="5">
-        <v>0.25310972127417664</v>
+        <v>0.33221498515308817</v>
       </c>
       <c r="H102" s="5">
-        <v>0.30889843532311961</v>
+        <v>0.29967383614139992</v>
       </c>
       <c r="J102" s="5">
-        <v>0.52769482274880508</v>
+        <v>0.26112624304449067</v>
       </c>
       <c r="K102" s="5">
-        <v>0.47100482906314012</v>
+        <v>0.73879431114698246</v>
       </c>
       <c r="L102" t="s">
         <v>20</v>
@@ -27826,19 +27826,19 @@
         <v>44486</v>
       </c>
       <c r="F103" s="5">
-        <v>0.42136572184724458</v>
+        <v>0.42650552675344111</v>
       </c>
       <c r="G103" s="5">
-        <v>0.23512366523012274</v>
+        <v>0.2316325848093132</v>
       </c>
       <c r="H103" s="5">
-        <v>0.31947095879817577</v>
+        <v>0.31807443474182678</v>
       </c>
       <c r="J103" s="5">
-        <v>0.61776637367782916</v>
+        <v>0.63541937083264588</v>
       </c>
       <c r="K103" s="5">
-        <v>0.3794405675801909</v>
+        <v>0.36130822969849619</v>
       </c>
       <c r="L103" t="s">
         <v>11</v>
@@ -27876,19 +27876,19 @@
         <v>44486</v>
       </c>
       <c r="F104" s="5">
-        <v>0.60950899837448291</v>
+        <v>0.70726002431138224</v>
       </c>
       <c r="G104" s="5">
-        <v>0.21788565834277929</v>
+        <v>0.17420402229739312</v>
       </c>
       <c r="H104" s="5">
-        <v>0.16509402042520965</v>
+        <v>0.11077120455255957</v>
       </c>
       <c r="J104" s="5">
-        <v>0.54665355206871447</v>
+        <v>0.63933753682204442</v>
       </c>
       <c r="K104" s="5">
-        <v>0.44925956926247845</v>
+        <v>0.34715056429631774</v>
       </c>
       <c r="L104" t="s">
         <v>16</v>
@@ -27926,19 +27926,19 @@
         <v>44486</v>
       </c>
       <c r="F105" s="5">
-        <v>0.48876077308823512</v>
+        <v>0.19480270436288175</v>
       </c>
       <c r="G105" s="5">
-        <v>0.31415390937329762</v>
+        <v>0.27887034217263673</v>
       </c>
       <c r="H105" s="5">
-        <v>0.19053600438419396</v>
+        <v>0.47232268912279435</v>
       </c>
       <c r="J105" s="5">
-        <v>0.26330796575852378</v>
+        <v>0.34687507211065299</v>
       </c>
       <c r="K105" s="5">
-        <v>0.73648444216935749</v>
+        <v>0.65255762982492305</v>
       </c>
       <c r="L105" t="s">
         <v>20</v>
@@ -27976,19 +27976,19 @@
         <v>44486</v>
       </c>
       <c r="F106" s="5">
-        <v>0.29424222426047403</v>
+        <v>0.38385642974157858</v>
       </c>
       <c r="G106" s="5">
-        <v>0.20422915562076605</v>
+        <v>0.21521710199459371</v>
       </c>
       <c r="H106" s="5">
-        <v>0.45666998569732092</v>
+        <v>0.3703435440192564</v>
       </c>
       <c r="J106" s="5">
-        <v>0.74018125619072683</v>
+        <v>0.72534012596934039</v>
       </c>
       <c r="K106" s="5">
-        <v>0.25007533091841061</v>
+        <v>0.26770119968717559</v>
       </c>
       <c r="L106" t="s">
         <v>11</v>
@@ -28026,22 +28026,22 @@
         <v>44486</v>
       </c>
       <c r="F107" s="5">
-        <v>0.56357103939439401</v>
+        <v>0.80156209826566005</v>
       </c>
       <c r="G107" s="5">
-        <v>0.27955049221434902</v>
+        <v>0.13455188864861353</v>
       </c>
       <c r="H107" s="5">
-        <v>0.15245591821122034</v>
+        <v>5.3712011012291179E-2</v>
       </c>
       <c r="J107" s="5">
-        <v>0.31160893046578841</v>
+        <v>0.6143807932998897</v>
       </c>
       <c r="K107" s="5">
-        <v>0.68782340990681146</v>
+        <v>0.36490629725793783</v>
       </c>
       <c r="L107" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="N107" s="5">
         <v>0.56357103939439401</v>
@@ -28076,22 +28076,22 @@
         <v>44486</v>
       </c>
       <c r="F108" s="5">
-        <v>0.73986736939514675</v>
+        <v>0.29827543064286605</v>
       </c>
       <c r="G108" s="5">
-        <v>0.16443474940212557</v>
+        <v>0.27829801161479906</v>
       </c>
       <c r="H108" s="5">
-        <v>8.8836306547268748E-2</v>
+        <v>0.38805544924051855</v>
       </c>
       <c r="J108" s="5">
-        <v>0.61244929330591447</v>
+        <v>0.4132880371627396</v>
       </c>
       <c r="K108" s="5">
-        <v>0.37382355805946388</v>
+        <v>0.58620853610898838</v>
       </c>
       <c r="L108" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="N108" s="5">
         <v>0.73986736939514675</v>
@@ -28126,22 +28126,22 @@
         <v>44486</v>
       </c>
       <c r="F109" s="5">
-        <v>2.0197143673851326E-2</v>
+        <v>0.49375610833650702</v>
       </c>
       <c r="G109" s="5">
-        <v>0.14345143180362241</v>
+        <v>0.25977551437670093</v>
       </c>
       <c r="H109" s="5">
-        <v>0.66931208551414834</v>
+        <v>0.23359311114078318</v>
       </c>
       <c r="J109" s="5">
-        <v>0.38066102828662984</v>
+        <v>0.4565488177336951</v>
       </c>
       <c r="K109" s="5">
-        <v>0.6137191639123899</v>
+        <v>0.54238861436805919</v>
       </c>
       <c r="L109" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="N109" s="5">
         <v>2.0197143673851326E-2</v>
@@ -28176,22 +28176,22 @@
         <v>44486</v>
       </c>
       <c r="F110" s="5">
-        <v>0.13337871946571059</v>
+        <v>0.31080490307259528</v>
       </c>
       <c r="G110" s="5">
-        <v>0.20694373355796677</v>
+        <v>0.28277886857798895</v>
       </c>
       <c r="H110" s="5">
-        <v>0.57174520131999429</v>
+        <v>0.3738916869288772</v>
       </c>
       <c r="J110" s="5">
-        <v>0.50168845714581956</v>
+        <v>0.40147930915395774</v>
       </c>
       <c r="K110" s="5">
-        <v>0.49428122275649311</v>
+        <v>0.59809945577465795</v>
       </c>
       <c r="L110" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="N110" s="5">
         <v>0.13337871946571059</v>
@@ -28226,22 +28226,22 @@
         <v>44486</v>
       </c>
       <c r="F111" s="5">
-        <v>0.11543975368895416</v>
+        <v>0.44930090507904491</v>
       </c>
       <c r="G111" s="5">
-        <v>0.16576762185311308</v>
+        <v>0.22640911731128277</v>
       </c>
       <c r="H111" s="5">
-        <v>0.61823952576571528</v>
+        <v>0.30251280977023748</v>
       </c>
       <c r="J111" s="5">
-        <v>0.63504770135025523</v>
+        <v>0.65748487086557039</v>
       </c>
       <c r="K111" s="5">
-        <v>0.35194314347707795</v>
+        <v>0.33834901421649233</v>
       </c>
       <c r="L111" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="N111" s="5">
         <v>0.11543975368895416</v>
@@ -28276,22 +28276,22 @@
         <v>44486</v>
       </c>
       <c r="F112" s="5">
-        <v>0.33584199803130399</v>
+        <v>0.28698157885299141</v>
       </c>
       <c r="G112" s="5">
-        <v>0.20021672931095236</v>
+        <v>0.2221626541407774</v>
       </c>
       <c r="H112" s="5">
-        <v>0.42457900840622054</v>
+        <v>0.44590217101782414</v>
       </c>
       <c r="J112" s="5">
-        <v>0.78413429630860332</v>
+        <v>0.64713031637204665</v>
       </c>
       <c r="K112" s="5">
-        <v>0.20254417857141302</v>
+        <v>0.34848891554381883</v>
       </c>
       <c r="L112" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="N112" s="5">
         <v>0.33584199803130399</v>
@@ -28326,22 +28326,22 @@
         <v>44486</v>
       </c>
       <c r="F113" s="5">
-        <v>0.28795102945099271</v>
+        <v>0.70902818399379075</v>
       </c>
       <c r="G113" s="5">
-        <v>0.21133374214359762</v>
+        <v>0.17214448912270919</v>
       </c>
       <c r="H113" s="5">
-        <v>0.45531421458079491</v>
+        <v>0.11043723770321408</v>
       </c>
       <c r="J113" s="5">
-        <v>0.70086991546683552</v>
+        <v>0.65113467465304165</v>
       </c>
       <c r="K113" s="5">
-        <v>0.29215616728497185</v>
+        <v>0.33404455162897462</v>
       </c>
       <c r="L113" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="N113" s="5">
         <v>0.28795102945099271</v>
@@ -28376,22 +28376,22 @@
         <v>44486</v>
       </c>
       <c r="F114" s="5">
-        <v>0.43543741278453679</v>
+        <v>0.24583017469849464</v>
       </c>
       <c r="G114" s="5">
-        <v>0.18598309077126221</v>
+        <v>0.24907472764542807</v>
       </c>
       <c r="H114" s="5">
-        <v>0.33777100460700504</v>
+        <v>0.454879226642668</v>
       </c>
       <c r="J114" s="5">
-        <v>0.85485132100126471</v>
+        <v>0.49270407469759081</v>
       </c>
       <c r="K114" s="5">
-        <v>0.11143831921117603</v>
+        <v>0.5058147148517449</v>
       </c>
       <c r="L114" t="s">
-        <v>408</v>
+        <v>28</v>
       </c>
       <c r="N114" s="5">
         <v>0.43543741278453679</v>
@@ -28426,22 +28426,22 @@
         <v>44486</v>
       </c>
       <c r="F115" s="5">
-        <v>0.86815410438222174</v>
+        <v>0.42239409277209022</v>
       </c>
       <c r="G115" s="5">
-        <v>8.5252781873053199E-2</v>
+        <v>0.27520889517994646</v>
       </c>
       <c r="H115" s="5">
-        <v>1.8406683727926223E-2</v>
+        <v>0.28377153698555507</v>
       </c>
       <c r="J115" s="5">
-        <v>0.63248408307160764</v>
+        <v>0.42764911450424908</v>
       </c>
       <c r="K115" s="5">
-        <v>0.32590367520292668</v>
+        <v>0.57178208387680773</v>
       </c>
       <c r="L115" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="N115" s="5">
         <v>0.86815410438222174</v>
@@ -28476,22 +28476,22 @@
         <v>44486</v>
       </c>
       <c r="F116" s="5">
-        <v>0.62579710485793827</v>
+        <v>0.72992122111454016</v>
       </c>
       <c r="G116" s="5">
-        <v>0.31371623934836507</v>
+        <v>0.15785659068725991</v>
       </c>
       <c r="H116" s="5">
-        <v>6.013273309709171E-2</v>
+        <v>9.8965427928443581E-2</v>
       </c>
       <c r="J116" s="5">
-        <v>0.16103727913079477</v>
+        <v>0.70319413375846196</v>
       </c>
       <c r="K116" s="5">
-        <v>0.83873150108384653</v>
+        <v>0.27189926756645588</v>
       </c>
       <c r="L116" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="N116" s="5">
         <v>0.62579710485793827</v>
@@ -28526,22 +28526,22 @@
         <v>44486</v>
       </c>
       <c r="F117" s="5">
-        <v>0.56190293487995191</v>
+        <v>0.28788828350288997</v>
       </c>
       <c r="G117" s="5">
-        <v>0.25413859780813736</v>
+        <v>0.2418960130393652</v>
       </c>
       <c r="H117" s="5">
-        <v>0.17682080523792168</v>
+        <v>0.4271368074244698</v>
       </c>
       <c r="J117" s="5">
-        <v>0.41666363416758567</v>
+        <v>0.55493355794525456</v>
       </c>
       <c r="K117" s="5">
-        <v>0.58209812913279102</v>
+        <v>0.44309310210530034</v>
       </c>
       <c r="L117" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="N117" s="5">
         <v>0.56190293487995191</v>
@@ -28576,22 +28576,22 @@
         <v>44486</v>
       </c>
       <c r="F118" s="5">
-        <v>0.67358013705416664</v>
+        <v>0.34057142606960544</v>
       </c>
       <c r="G118" s="5">
-        <v>0.1824690964955219</v>
+        <v>0.3779289382112288</v>
       </c>
       <c r="H118" s="5">
-        <v>0.13474468122787037</v>
+        <v>0.26980366063791683</v>
       </c>
       <c r="J118" s="5">
-        <v>0.6660052676522118</v>
+        <v>0.17311475249269076</v>
       </c>
       <c r="K118" s="5">
-        <v>0.32063824582995037</v>
+        <v>0.82686351128403768</v>
       </c>
       <c r="L118" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="N118" s="5">
         <v>0.67358013705416664</v>
@@ -28626,22 +28626,22 @@
         <v>44486</v>
       </c>
       <c r="F119" s="5">
-        <v>0</v>
+        <v>0.5935604591928676</v>
       </c>
       <c r="G119" s="5">
-        <v>1</v>
+        <v>0.21547523689903045</v>
       </c>
       <c r="H119" s="5">
-        <v>0</v>
+        <v>0.18168598588351764</v>
       </c>
       <c r="J119" s="5">
-        <v>0</v>
+        <v>0.58888790027261706</v>
       </c>
       <c r="K119" s="5">
-        <v>1</v>
+        <v>0.40616457365152164</v>
       </c>
       <c r="L119" t="s">
-        <v>133</v>
+        <v>16</v>
       </c>
       <c r="N119" s="5">
         <v>0</v>
@@ -28676,22 +28676,22 @@
         <v>44486</v>
       </c>
       <c r="F120" s="5">
-        <v>0.53517269352544494</v>
+        <v>0.38221479209771808</v>
       </c>
       <c r="G120" s="5">
-        <v>0.22368777842491669</v>
+        <v>0.24045787226877116</v>
       </c>
       <c r="H120" s="5">
-        <v>0.22767465137411175</v>
+        <v>0.34887547533162377</v>
       </c>
       <c r="J120" s="5">
-        <v>0.61356094423756935</v>
+        <v>0.59360045905067249</v>
       </c>
       <c r="K120" s="5">
-        <v>0.3821796525405044</v>
+        <v>0.40422490624366825</v>
       </c>
       <c r="L120" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="N120" s="5">
         <v>0.53517269352544494</v>
@@ -28726,22 +28726,22 @@
         <v>44486</v>
       </c>
       <c r="F121" s="5">
-        <v>0.1461064916176365</v>
+        <v>0.5975372785221198</v>
       </c>
       <c r="G121" s="5">
-        <v>0.4010227990467149</v>
+        <v>0.22855309278858271</v>
       </c>
       <c r="H121" s="5">
-        <v>0.42292994247836041</v>
+        <v>0.16677892178422796</v>
       </c>
       <c r="J121" s="5">
-        <v>0.11784153703550826</v>
+        <v>0.50135766769814738</v>
       </c>
       <c r="K121" s="5">
-        <v>0.88213057076666912</v>
+        <v>0.49583712291658621</v>
       </c>
       <c r="L121" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="N121" s="5">
         <v>0.1461064916176365</v>
@@ -28775,23 +28775,23 @@
       <c r="D122" s="4">
         <v>44486</v>
       </c>
-      <c r="F122" s="5">
-        <v>0.28712079798555401</v>
-      </c>
-      <c r="G122" s="5">
-        <v>0.43447541692199737</v>
-      </c>
-      <c r="H122" s="5">
-        <v>0.26902616541544727</v>
-      </c>
-      <c r="J122" s="5">
-        <v>0.10587800132303506</v>
-      </c>
-      <c r="K122" s="5">
-        <v>0.89411750692836922</v>
-      </c>
-      <c r="L122" t="s">
-        <v>20</v>
+      <c r="F122" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G122" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H122" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J122" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K122" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L122" t="e">
+        <v>#N/A</v>
       </c>
       <c r="N122" s="5">
         <v>0.28712079798555401</v>
@@ -28826,22 +28826,22 @@
         <v>44486</v>
       </c>
       <c r="F123" s="5">
-        <v>0.40350815324169048</v>
+        <v>0.51658376431233266</v>
       </c>
       <c r="G123" s="5">
-        <v>0.34950963625138265</v>
+        <v>0.23966517758905312</v>
       </c>
       <c r="H123" s="5">
-        <v>0.2373495628519362</v>
+        <v>0.23057417515807441</v>
       </c>
       <c r="J123" s="5">
-        <v>0.2142508437957604</v>
+        <v>0.53912852598113536</v>
       </c>
       <c r="K123" s="5">
-        <v>0.78568906531961857</v>
+        <v>0.4586295578875611</v>
       </c>
       <c r="L123" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="N123" s="5">
         <v>0.40350815324169048</v>
@@ -28876,22 +28876,22 @@
         <v>44486</v>
       </c>
       <c r="F124" s="5">
-        <v>7.7856578200658291E-2</v>
+        <v>0.33076747945051055</v>
       </c>
       <c r="G124" s="5">
-        <v>0.18596609274850334</v>
+        <v>0.26155480289384553</v>
       </c>
       <c r="H124" s="5">
-        <v>0.61994992696258144</v>
+        <v>0.37446658782829234</v>
       </c>
       <c r="J124" s="5">
-        <v>0.4444698164535596</v>
+        <v>0.48830305944240393</v>
       </c>
       <c r="K124" s="5">
-        <v>0.55105375680937696</v>
+        <v>0.5107857148185766</v>
       </c>
       <c r="L124" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="N124" s="5">
         <v>7.7856578200658291E-2</v>
@@ -28926,22 +28926,22 @@
         <v>44486</v>
       </c>
       <c r="F125" s="5">
-        <v>0.6356047763949676</v>
+        <v>0.75521124461344435</v>
       </c>
       <c r="G125" s="5">
-        <v>0.19305613456276452</v>
+        <v>0.15354230235265823</v>
       </c>
       <c r="H125" s="5">
-        <v>0.16122700401139614</v>
+        <v>8.1640617028971241E-2</v>
       </c>
       <c r="J125" s="5">
-        <v>0.67038025758195841</v>
+        <v>0.65022097328536066</v>
       </c>
       <c r="K125" s="5">
-        <v>0.31852512942540151</v>
+        <v>0.33018307436144767</v>
       </c>
       <c r="L125" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="N125" s="5">
         <v>0.6356047763949676</v>
@@ -28976,22 +28976,22 @@
         <v>44486</v>
       </c>
       <c r="F126" s="5">
-        <v>0.16470613933655151</v>
+        <v>0.26995030389378738</v>
       </c>
       <c r="G126" s="5">
-        <v>0.53224212878940891</v>
+        <v>0.22432236470555836</v>
       </c>
       <c r="H126" s="5">
-        <v>0.29463693218406056</v>
+        <v>0.45757629271183331</v>
       </c>
       <c r="J126" s="5">
-        <v>4.2193740608185093E-2</v>
+        <v>0.62290302577260026</v>
       </c>
       <c r="K126" s="5">
-        <v>0.95780550420960997</v>
+        <v>0.37321642357964085</v>
       </c>
       <c r="L126" t="s">
-        <v>133</v>
+        <v>28</v>
       </c>
       <c r="N126" s="5">
         <v>0.16470613933655151</v>
@@ -29026,19 +29026,19 @@
         <v>44486</v>
       </c>
       <c r="F127" s="5">
-        <v>0.20959875642968834</v>
+        <v>0.16612677927842712</v>
       </c>
       <c r="G127" s="5">
-        <v>0.23940572403777619</v>
+        <v>0.25097646959947234</v>
       </c>
       <c r="H127" s="5">
-        <v>0.49117080023300658</v>
+        <v>0.51499771594508004</v>
       </c>
       <c r="J127" s="5">
-        <v>0.49466650177257754</v>
+        <v>0.39971018728048924</v>
       </c>
       <c r="K127" s="5">
-        <v>0.50335275895205411</v>
+        <v>0.59903545713090967</v>
       </c>
       <c r="L127" t="s">
         <v>28</v>
@@ -29076,22 +29076,22 @@
         <v>44486</v>
       </c>
       <c r="F128" s="5">
-        <v>0.48403679217065659</v>
+        <v>0.75401927373241151</v>
       </c>
       <c r="G128" s="5">
-        <v>0.29360821361323142</v>
+        <v>0.16086863963872644</v>
       </c>
       <c r="H128" s="5">
-        <v>0.21301289139711693</v>
+        <v>7.8948556265766079E-2</v>
       </c>
       <c r="J128" s="5">
-        <v>0.32857658406710344</v>
+        <v>0.58920282602206864</v>
       </c>
       <c r="K128" s="5">
-        <v>0.67106610100186204</v>
+        <v>0.39794182508910503</v>
       </c>
       <c r="L128" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="N128" s="5">
         <v>0.48403679217065659</v>
@@ -29126,22 +29126,22 @@
         <v>44486</v>
       </c>
       <c r="F129" s="5">
-        <v>0.76017192059880634</v>
+        <v>0.53453615055196502</v>
       </c>
       <c r="G129" s="5">
-        <v>0.17894073159274101</v>
+        <v>0.24806663595557207</v>
       </c>
       <c r="H129" s="5">
-        <v>5.8562532113774934E-2</v>
+        <v>0.20705121859961445</v>
       </c>
       <c r="J129" s="5">
-        <v>0.42413685366165604</v>
+        <v>0.47689866213456072</v>
       </c>
       <c r="K129" s="5">
-        <v>0.57115945068171026</v>
+        <v>0.52150809084390026</v>
       </c>
       <c r="L129" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
       <c r="N129" s="5">
         <v>0.76017192059880634</v>
@@ -29176,22 +29176,22 @@
         <v>44486</v>
       </c>
       <c r="F130" s="5">
-        <v>0.38522972715706838</v>
+        <v>0.61821620503674568</v>
       </c>
       <c r="G130" s="5">
-        <v>0.43677188441875914</v>
+        <v>0.25421009138421807</v>
       </c>
       <c r="H130" s="5">
-        <v>0.17488522867751535</v>
+        <v>0.12449579489595637</v>
       </c>
       <c r="J130" s="5">
-        <v>9.5190666413655853E-2</v>
+        <v>0.34219142454413742</v>
       </c>
       <c r="K130" s="5">
-        <v>0.90480048683863268</v>
+        <v>0.65674501491005832</v>
       </c>
       <c r="L130" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="N130" s="5">
         <v>0.38522972715706838</v>
@@ -29226,22 +29226,22 @@
         <v>44486</v>
       </c>
       <c r="F131" s="5">
-        <v>0.78038360546533903</v>
+        <v>0.31994119175132163</v>
       </c>
       <c r="G131" s="5">
-        <v>0.21861601122222807</v>
+        <v>0.28371516873092006</v>
       </c>
       <c r="H131" s="5">
-        <v>0</v>
+        <v>0.36538891206484636</v>
       </c>
       <c r="J131" s="5">
-        <v>0.19530047735354825</v>
+        <v>0.40043956771287714</v>
       </c>
       <c r="K131" s="5">
-        <v>0.80369913933401882</v>
+        <v>0.59915786477556721</v>
       </c>
       <c r="L131" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="N131" s="5">
         <v>0.78038360546533903</v>
@@ -29276,22 +29276,22 @@
         <v>44486</v>
       </c>
       <c r="F132" s="5">
-        <v>0.87564178694631667</v>
+        <v>0.65895194514826039</v>
       </c>
       <c r="G132" s="5">
-        <v>4.1162731526624086E-2</v>
+        <v>0.195324018418364</v>
       </c>
       <c r="H132" s="5">
-        <v>3.3954686565209023E-3</v>
+        <v>0.13871968555935563</v>
       </c>
       <c r="J132" s="5">
-        <v>0.65989061946866256</v>
+        <v>0.60242046073176436</v>
       </c>
       <c r="K132" s="5">
-        <v>0.24981747188468698</v>
+        <v>0.38965262940245543</v>
       </c>
       <c r="L132" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="N132" s="5">
         <v>0.87564178694631667</v>
@@ -29326,22 +29326,22 @@
         <v>44486</v>
       </c>
       <c r="F133" s="5">
-        <v>0.68249959383393377</v>
+        <v>0.50463624193328194</v>
       </c>
       <c r="G133" s="5">
-        <v>0.20146894992309683</v>
+        <v>0.2660990472175519</v>
       </c>
       <c r="H133" s="5">
-        <v>0.1120309414802588</v>
+        <v>0.21833501641651681</v>
       </c>
       <c r="J133" s="5">
-        <v>0.50031601606487297</v>
+        <v>0.41954047884684859</v>
       </c>
       <c r="K133" s="5">
-        <v>0.49497306725960932</v>
+        <v>0.57960038187414264</v>
       </c>
       <c r="L133" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="N133" s="5">
         <v>0.68249959383393377</v>
@@ -29426,22 +29426,22 @@
         <v>44486</v>
       </c>
       <c r="F135" s="5">
-        <v>0.26834575019491763</v>
+        <v>0.15522623935480476</v>
       </c>
       <c r="G135" s="5">
-        <v>0.22099892836083909</v>
+        <v>0.30741086214181212</v>
       </c>
       <c r="H135" s="5">
-        <v>0.4619611762767793</v>
+        <v>0.4839077733160273</v>
       </c>
       <c r="J135" s="5">
-        <v>0.63734553418472395</v>
+        <v>0.24783675230990382</v>
       </c>
       <c r="K135" s="5">
-        <v>0.35823111387674184</v>
+        <v>0.7518950142467189</v>
       </c>
       <c r="L135" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="N135" s="5">
         <v>0.26834575019491763</v>
@@ -29576,22 +29576,22 @@
         <v>44486</v>
       </c>
       <c r="F138" s="5">
-        <v>0.26120278938996294</v>
+        <v>0.35405886994956004</v>
       </c>
       <c r="G138" s="5">
-        <v>0.59027395582648268</v>
+        <v>0.25656482672725672</v>
       </c>
       <c r="H138" s="5">
-        <v>0.14737467180846817</v>
+        <v>0.35891294958885966</v>
       </c>
       <c r="J138" s="5">
-        <v>2.4537169099802712E-2</v>
+        <v>0.51459130173061052</v>
       </c>
       <c r="K138" s="5">
-        <v>0.97546266008538596</v>
+        <v>0.48430419500359528</v>
       </c>
       <c r="L138" t="s">
-        <v>133</v>
+        <v>20</v>
       </c>
       <c r="N138" s="5">
         <v>0.26120278938996294</v>
@@ -29626,22 +29626,22 @@
         <v>44486</v>
       </c>
       <c r="F139" s="5">
-        <v>0.42431916263885133</v>
+        <v>0.57166736006752428</v>
       </c>
       <c r="G139" s="5">
-        <v>0.27816573709302211</v>
+        <v>0.29337302448677494</v>
       </c>
       <c r="H139" s="5">
-        <v>0.27957874871367727</v>
+        <v>0.13210383806534653</v>
       </c>
       <c r="J139" s="5">
-        <v>0.41515481266211923</v>
+        <v>0.25921170347463768</v>
       </c>
       <c r="K139" s="5">
-        <v>0.58433064713248251</v>
+        <v>0.74039790950758233</v>
       </c>
       <c r="L139" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="N139" s="5">
         <v>0.42431916263885133</v>
@@ -29675,23 +29675,23 @@
       <c r="D140" s="4">
         <v>44486</v>
       </c>
-      <c r="F140" s="5">
-        <v>0.6059607132652336</v>
-      </c>
-      <c r="G140" s="5">
-        <v>0.3174477010770449</v>
-      </c>
-      <c r="H140" s="5">
-        <v>7.6001431575254255E-2</v>
-      </c>
-      <c r="J140" s="5">
-        <v>0.17003364443128047</v>
-      </c>
-      <c r="K140" s="5">
-        <v>0.82974845942139186</v>
-      </c>
-      <c r="L140" t="s">
-        <v>17</v>
+      <c r="F140" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G140" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H140" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J140" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K140" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L140" t="e">
+        <v>#N/A</v>
       </c>
       <c r="N140" s="5">
         <v>0.6059607132652336</v>
@@ -29776,22 +29776,22 @@
         <v>44486</v>
       </c>
       <c r="F142" s="5">
-        <v>0.48018554948326203</v>
+        <v>0.53310068727400062</v>
       </c>
       <c r="G142" s="5">
-        <v>0.25384269035818918</v>
+        <v>0.27854007859662994</v>
       </c>
       <c r="H142" s="5">
-        <v>0.25086388210196503</v>
+        <v>0.18154341268262916</v>
       </c>
       <c r="J142" s="5">
-        <v>0.49457936293813859</v>
+        <v>0.34459946043392681</v>
       </c>
       <c r="K142" s="5">
-        <v>0.50410791677031375</v>
+        <v>0.65481248351193155</v>
       </c>
       <c r="L142" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="N142" s="5">
         <v>0.48018554948326203</v>
@@ -29826,22 +29826,22 @@
         <v>44486</v>
       </c>
       <c r="F143" s="5">
-        <v>0.37759160787533474</v>
+        <v>0.6189614481990634</v>
       </c>
       <c r="G143" s="5">
-        <v>0.3792981226719877</v>
+        <v>0.27248333171602912</v>
       </c>
       <c r="H143" s="5">
-        <v>0.23479687909609012</v>
+        <v>0.10669540649784655</v>
       </c>
       <c r="J143" s="5">
-        <v>0.16634647634230942</v>
+        <v>0.2734744139956492</v>
       </c>
       <c r="K143" s="5">
-        <v>0.83362789266302306</v>
+        <v>0.72589792554450083</v>
       </c>
       <c r="L143" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="N143" s="5">
         <v>0.37759160787533474</v>
@@ -29876,22 +29876,22 @@
         <v>44486</v>
       </c>
       <c r="F144" s="5">
-        <v>0.62143180572491019</v>
+        <v>0.34463594399641778</v>
       </c>
       <c r="G144" s="5">
-        <v>0.37849849519541306</v>
+        <v>0.33463246486981502</v>
       </c>
       <c r="H144" s="5">
-        <v>0</v>
+        <v>0.30277409995388299</v>
       </c>
       <c r="J144" s="5">
-        <v>7.5072536408493165E-2</v>
+        <v>0.25576613612181287</v>
       </c>
       <c r="K144" s="5">
-        <v>0.9248577645118301</v>
+        <v>0.74416052015535283</v>
       </c>
       <c r="L144" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="N144" s="5">
         <v>0.62143180572491019</v>
@@ -29975,23 +29975,23 @@
       <c r="D146" s="4">
         <v>44486</v>
       </c>
-      <c r="F146" s="5">
-        <v>0.26116647275229421</v>
-      </c>
-      <c r="G146" s="5">
-        <v>0.47652241561627945</v>
-      </c>
-      <c r="H146" s="5">
-        <v>0.25522889309105162</v>
-      </c>
-      <c r="J146" s="5">
-        <v>7.2964391106712781E-2</v>
-      </c>
-      <c r="K146" s="5">
-        <v>0.927034083484232</v>
-      </c>
-      <c r="L146" t="s">
-        <v>133</v>
+      <c r="F146" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G146" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H146" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J146" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K146" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L146" t="e">
+        <v>#N/A</v>
       </c>
       <c r="N146" s="5">
         <v>0.26116647275229421</v>
@@ -30026,22 +30026,22 @@
         <v>44486</v>
       </c>
       <c r="F147" s="5">
-        <v>0.52909340854477716</v>
+        <v>0.39954478542678257</v>
       </c>
       <c r="G147" s="5">
-        <v>0.24608102853547964</v>
+        <v>0.26220875511320135</v>
       </c>
       <c r="H147" s="5">
-        <v>0.21370351923821521</v>
+        <v>0.31480496627962329</v>
       </c>
       <c r="J147" s="5">
-        <v>0.49269512533823784</v>
+        <v>0.48875726528972668</v>
       </c>
       <c r="K147" s="5">
-        <v>0.50557957686397226</v>
+        <v>0.51034478494023316</v>
       </c>
       <c r="L147" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="N147" s="5">
         <v>0.52909340854477716</v>
@@ -30076,22 +30076,22 @@
         <v>44486</v>
       </c>
       <c r="F148" s="5">
-        <v>0.30102529871733541</v>
+        <v>0.68547509510808524</v>
       </c>
       <c r="G148" s="5">
-        <v>0.40540454443177687</v>
+        <v>0.19230774018644642</v>
       </c>
       <c r="H148" s="5">
-        <v>0.2818769360657446</v>
+        <v>0.11703908303083209</v>
       </c>
       <c r="J148" s="5">
-        <v>0.13675808116956914</v>
+        <v>0.55794830021910125</v>
       </c>
       <c r="K148" s="5">
-        <v>0.86323224528597553</v>
+        <v>0.43511471632637944</v>
       </c>
       <c r="L148" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="N148" s="5">
         <v>0.30102529871733541</v>
@@ -30126,22 +30126,22 @@
         <v>44486</v>
       </c>
       <c r="F149" s="5">
-        <v>0.27287945328766677</v>
+        <v>0.1505987111803066</v>
       </c>
       <c r="G149" s="5">
-        <v>0.3195428697089458</v>
+        <v>0.21534491505546738</v>
       </c>
       <c r="H149" s="5">
-        <v>0.37712450364805372</v>
+        <v>0.55360855088467142</v>
       </c>
       <c r="J149" s="5">
-        <v>0.28343478654124421</v>
+        <v>0.50226057875044616</v>
       </c>
       <c r="K149" s="5">
-        <v>0.71643108135716493</v>
+        <v>0.49427341903619071</v>
       </c>
       <c r="L149" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="N149" s="5">
         <v>0.27287945328766677</v>
@@ -30176,22 +30176,22 @@
         <v>44486</v>
       </c>
       <c r="F150" s="5">
-        <v>0.51768935826493123</v>
+        <v>0.66364712239544743</v>
       </c>
       <c r="G150" s="5">
-        <v>0.29551579519085569</v>
+        <v>0.2141665850590217</v>
       </c>
       <c r="H150" s="5">
-        <v>0.18055949349174905</v>
+        <v>0.11838698634062816</v>
       </c>
       <c r="J150" s="5">
-        <v>0.29880751864764743</v>
+        <v>0.46313762302391259</v>
       </c>
       <c r="K150" s="5">
-        <v>0.70083290269343246</v>
+        <v>0.53356535949861694</v>
       </c>
       <c r="L150" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="N150" s="5">
         <v>0.51768935826493123</v>
@@ -30226,22 +30226,22 @@
         <v>44486</v>
       </c>
       <c r="F151" s="5">
-        <v>0.77284923488391477</v>
+        <v>0.40750275999600505</v>
       </c>
       <c r="G151" s="5">
-        <v>0.22627312311750505</v>
+        <v>0.37779688536069223</v>
       </c>
       <c r="H151" s="5">
-        <v>0</v>
+        <v>0.20847475479345323</v>
       </c>
       <c r="J151" s="5">
-        <v>0.18677263978853273</v>
+        <v>0.1624852225691453</v>
       </c>
       <c r="K151" s="5">
-        <v>0.81234971821288715</v>
+        <v>0.83748241178369465</v>
       </c>
       <c r="L151" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="N151" s="5">
         <v>0.77284923488391477</v>
@@ -30275,23 +30275,23 @@
       <c r="D152" s="4">
         <v>44486</v>
       </c>
-      <c r="F152" s="5">
-        <v>0.76731579883775558</v>
-      </c>
-      <c r="G152" s="5">
-        <v>0.20147280279332588</v>
-      </c>
-      <c r="H152" s="5">
-        <v>3.0056799984208633E-2</v>
-      </c>
-      <c r="J152" s="5">
-        <v>0.28288837419280471</v>
-      </c>
-      <c r="K152" s="5">
-        <v>0.71523524647496128</v>
-      </c>
-      <c r="L152" t="s">
-        <v>37</v>
+      <c r="F152" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G152" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H152" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J152" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K152" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L152" t="e">
+        <v>#N/A</v>
       </c>
       <c r="N152" s="5">
         <v>0.76731579883775558</v>
@@ -30326,22 +30326,22 @@
         <v>44486</v>
       </c>
       <c r="F153" s="5">
-        <v>0.51276251392047689</v>
+        <v>0.20175416458831641</v>
       </c>
       <c r="G153" s="5">
-        <v>0.34152118987200841</v>
+        <v>0.19252756099938451</v>
       </c>
       <c r="H153" s="5">
-        <v>0.14295461602573495</v>
+        <v>0.53943343647901432</v>
       </c>
       <c r="J153" s="5">
-        <v>0.18562405186257439</v>
+        <v>0.69194212864819693</v>
       </c>
       <c r="K153" s="5">
-        <v>0.81425838908082449</v>
+        <v>0.29759569980498846</v>
       </c>
       <c r="L153" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="N153" s="5">
         <v>0.51276251392047689</v>
@@ -30375,23 +30375,23 @@
       <c r="D154" s="4">
         <v>44486</v>
       </c>
-      <c r="F154" s="5">
-        <v>0.72982407479720601</v>
-      </c>
-      <c r="G154" s="5">
-        <v>0.17791329967853381</v>
-      </c>
-      <c r="H154" s="5">
-        <v>8.8084107712461057E-2</v>
-      </c>
-      <c r="J154" s="5">
-        <v>0.5347663755143951</v>
-      </c>
-      <c r="K154" s="5">
-        <v>0.45740772225126197</v>
-      </c>
-      <c r="L154" t="s">
-        <v>16</v>
+      <c r="F154" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="G154" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="H154" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J154" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="K154" s="5" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="L154" t="e">
+        <v>#N/A</v>
       </c>
       <c r="N154" s="5">
         <v>0.72982407479720601</v>
@@ -30426,22 +30426,22 @@
         <v>44487</v>
       </c>
       <c r="F155" s="5">
-        <v>0.79608684723976464</v>
+        <v>0.55145772018961536</v>
       </c>
       <c r="G155" s="5">
-        <v>0.1473863400973793</v>
+        <v>0.24476623572580311</v>
       </c>
       <c r="H155" s="5">
-        <v>5.1227863961525323E-2</v>
+        <v>0.1945980762483715</v>
       </c>
       <c r="J155" s="5">
-        <v>0.52349321784277547</v>
+        <v>0.47512760529351655</v>
       </c>
       <c r="K155" s="5">
-        <v>0.46547285331350696</v>
+        <v>0.52312089801646044</v>
       </c>
       <c r="L155" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
       <c r="N155" s="5">
         <v>0.79608684723976464</v>
@@ -30460,6 +30460,506 @@
       </c>
       <c r="T155" t="s">
         <v>37</v>
+      </c>
+    </row>
+    <row r="156" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="F156">
+        <v>0.5975372785221198</v>
+      </c>
+      <c r="G156">
+        <v>0.22855309278858271</v>
+      </c>
+      <c r="H156">
+        <v>0.16677892178422796</v>
+      </c>
+      <c r="J156">
+        <v>0.50135766769814738</v>
+      </c>
+      <c r="K156">
+        <v>0.49583712291658621</v>
+      </c>
+      <c r="L156" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="157" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="F157">
+        <v>0.28712079798555401</v>
+      </c>
+      <c r="G157">
+        <v>0.43447541692199737</v>
+      </c>
+      <c r="H157">
+        <v>0.26902616541544727</v>
+      </c>
+      <c r="J157">
+        <v>0.10587800132303506</v>
+      </c>
+      <c r="K157">
+        <v>0.89411750692836922</v>
+      </c>
+      <c r="L157" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="158" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="F158">
+        <v>0.38221479209771808</v>
+      </c>
+      <c r="G158">
+        <v>0.24045787226877116</v>
+      </c>
+      <c r="H158">
+        <v>0.34887547533162377</v>
+      </c>
+      <c r="J158">
+        <v>0.59360045905067249</v>
+      </c>
+      <c r="K158">
+        <v>0.40422490624366825</v>
+      </c>
+      <c r="L158" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="159" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="F159">
+        <v>0.51658376431233266</v>
+      </c>
+      <c r="G159">
+        <v>0.23966517758905312</v>
+      </c>
+      <c r="H159">
+        <v>0.23057417515807441</v>
+      </c>
+      <c r="J159">
+        <v>0.53912852598113536</v>
+      </c>
+      <c r="K159">
+        <v>0.4586295578875611</v>
+      </c>
+      <c r="L159" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="160" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="F160">
+        <v>0.65895194514826039</v>
+      </c>
+      <c r="G160">
+        <v>0.195324018418364</v>
+      </c>
+      <c r="H160">
+        <v>0.13871968555935563</v>
+      </c>
+      <c r="J160">
+        <v>0.60242046073176436</v>
+      </c>
+      <c r="K160">
+        <v>0.38965262940245543</v>
+      </c>
+      <c r="L160" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="161" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F161">
+        <v>0.26995030389378738</v>
+      </c>
+      <c r="G161">
+        <v>0.22432236470555836</v>
+      </c>
+      <c r="H161">
+        <v>0.45757629271183331</v>
+      </c>
+      <c r="J161">
+        <v>0.62290302577260026</v>
+      </c>
+      <c r="K161">
+        <v>0.37321642357964085</v>
+      </c>
+      <c r="L161" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="162" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F162">
+        <v>0.50463624193328194</v>
+      </c>
+      <c r="G162">
+        <v>0.2660990472175519</v>
+      </c>
+      <c r="H162">
+        <v>0.21833501641651681</v>
+      </c>
+      <c r="J162">
+        <v>0.41954047884684859</v>
+      </c>
+      <c r="K162">
+        <v>0.57960038187414264</v>
+      </c>
+      <c r="L162" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="163" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F163">
+        <v>0.75521124461344435</v>
+      </c>
+      <c r="G163">
+        <v>0.15354230235265823</v>
+      </c>
+      <c r="H163">
+        <v>8.1640617028971241E-2</v>
+      </c>
+      <c r="J163">
+        <v>0.65022097328536066</v>
+      </c>
+      <c r="K163">
+        <v>0.33018307436144767</v>
+      </c>
+      <c r="L163" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="164" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F164">
+        <v>0.5031093798122791</v>
+      </c>
+      <c r="G164">
+        <v>0.31322954679287429</v>
+      </c>
+      <c r="H164">
+        <v>0.17810036963875953</v>
+      </c>
+      <c r="J164">
+        <v>0.25700688360089935</v>
+      </c>
+      <c r="K164">
+        <v>0.74277250712845322</v>
+      </c>
+      <c r="L164" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="165" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F165">
+        <v>0.6189614481990634</v>
+      </c>
+      <c r="G165">
+        <v>0.27248333171602912</v>
+      </c>
+      <c r="H165">
+        <v>0.10669540649784655</v>
+      </c>
+      <c r="J165">
+        <v>0.2734744139956492</v>
+      </c>
+      <c r="K165">
+        <v>0.72589792554450083</v>
+      </c>
+      <c r="L165" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="166" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F166">
+        <v>0.6059607132652336</v>
+      </c>
+      <c r="G166">
+        <v>0.3174477010770449</v>
+      </c>
+      <c r="H166">
+        <v>7.6001431575254255E-2</v>
+      </c>
+      <c r="J166">
+        <v>0.17003364443128047</v>
+      </c>
+      <c r="K166">
+        <v>0.82974845942139186</v>
+      </c>
+      <c r="L166" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="167" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F167">
+        <v>0.21322310206847891</v>
+      </c>
+      <c r="G167">
+        <v>0.34912156573509728</v>
+      </c>
+      <c r="H167">
+        <v>0.40520987738572928</v>
+      </c>
+      <c r="J167">
+        <v>0.204451667022918</v>
+      </c>
+      <c r="K167">
+        <v>0.79547580690178799</v>
+      </c>
+      <c r="L167" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="168" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F168">
+        <v>0.35405886994956004</v>
+      </c>
+      <c r="G168">
+        <v>0.25656482672725672</v>
+      </c>
+      <c r="H168">
+        <v>0.35891294958885966</v>
+      </c>
+      <c r="J168">
+        <v>0.51459130173061052</v>
+      </c>
+      <c r="K168">
+        <v>0.48430419500359528</v>
+      </c>
+      <c r="L168" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="169" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F169">
+        <v>0.39954478542678257</v>
+      </c>
+      <c r="G169">
+        <v>0.26220875511320135</v>
+      </c>
+      <c r="H169">
+        <v>0.31480496627962329</v>
+      </c>
+      <c r="J169">
+        <v>0.48875726528972668</v>
+      </c>
+      <c r="K169">
+        <v>0.51034478494023316</v>
+      </c>
+      <c r="L169" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="170" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F170">
+        <v>0.72982407479720601</v>
+      </c>
+      <c r="G170">
+        <v>0.17791329967853381</v>
+      </c>
+      <c r="H170">
+        <v>8.8084107712461057E-2</v>
+      </c>
+      <c r="J170">
+        <v>0.5347663755143951</v>
+      </c>
+      <c r="K170">
+        <v>0.45740772225126197</v>
+      </c>
+      <c r="L170" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="171" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F171">
+        <v>0.68547509510808524</v>
+      </c>
+      <c r="G171">
+        <v>0.19230774018644642</v>
+      </c>
+      <c r="H171">
+        <v>0.11703908303083209</v>
+      </c>
+      <c r="J171">
+        <v>0.55794830021910125</v>
+      </c>
+      <c r="K171">
+        <v>0.43511471632637944</v>
+      </c>
+      <c r="L171" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="172" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F172">
+        <v>0.1505987111803066</v>
+      </c>
+      <c r="G172">
+        <v>0.21534491505546738</v>
+      </c>
+      <c r="H172">
+        <v>0.55360855088467142</v>
+      </c>
+      <c r="J172">
+        <v>0.50226057875044616</v>
+      </c>
+      <c r="K172">
+        <v>0.49427341903619071</v>
+      </c>
+      <c r="L172" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="173" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F173">
+        <v>0.55145772018961536</v>
+      </c>
+      <c r="G173">
+        <v>0.24476623572580311</v>
+      </c>
+      <c r="H173">
+        <v>0.1945980762483715</v>
+      </c>
+      <c r="J173">
+        <v>0.47512760529351655</v>
+      </c>
+      <c r="K173">
+        <v>0.52312089801646044</v>
+      </c>
+      <c r="L173" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="174" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F174">
+        <v>0.37923946433867717</v>
+      </c>
+      <c r="G174">
+        <v>0.29403133872633819</v>
+      </c>
+      <c r="H174">
+        <v>0.30586958254564717</v>
+      </c>
+      <c r="J174">
+        <v>0.36733918097014734</v>
+      </c>
+      <c r="K174">
+        <v>0.6323822697694782</v>
+      </c>
+      <c r="L174" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="175" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F175">
+        <v>0.10427606587729879</v>
+      </c>
+      <c r="G175">
+        <v>0.2607713465025146</v>
+      </c>
+      <c r="H175">
+        <v>0.55462644071996647</v>
+      </c>
+      <c r="J175">
+        <v>0.29112893350182112</v>
+      </c>
+      <c r="K175">
+        <v>0.70806451097710932</v>
+      </c>
+      <c r="L175" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="176" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F176">
+        <v>0.5935604591928676</v>
+      </c>
+      <c r="G176">
+        <v>0.21547523689903045</v>
+      </c>
+      <c r="H176">
+        <v>0.18168598588351764</v>
+      </c>
+      <c r="J176">
+        <v>0.58888790027261706</v>
+      </c>
+      <c r="K176">
+        <v>0.40616457365152164</v>
+      </c>
+      <c r="L176" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="177" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F177">
+        <v>0.33076747945051055</v>
+      </c>
+      <c r="G177">
+        <v>0.26155480289384553</v>
+      </c>
+      <c r="H177">
+        <v>0.37446658782829234</v>
+      </c>
+      <c r="J177">
+        <v>0.48830305944240393</v>
+      </c>
+      <c r="K177">
+        <v>0.5107857148185766</v>
+      </c>
+      <c r="L177" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="178" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F178">
+        <v>0.75401927373241151</v>
+      </c>
+      <c r="G178">
+        <v>0.16086863963872644</v>
+      </c>
+      <c r="H178">
+        <v>7.8948556265766079E-2</v>
+      </c>
+      <c r="J178">
+        <v>0.58920282602206864</v>
+      </c>
+      <c r="K178">
+        <v>0.39794182508910503</v>
+      </c>
+      <c r="L178" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="179" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F179">
+        <v>0.66364712239544743</v>
+      </c>
+      <c r="G179">
+        <v>0.2141665850590217</v>
+      </c>
+      <c r="H179">
+        <v>0.11838698634062816</v>
+      </c>
+      <c r="J179">
+        <v>0.46313762302391259</v>
+      </c>
+      <c r="K179">
+        <v>0.53356535949861694</v>
+      </c>
+      <c r="L179" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="180" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F180">
+        <v>0.49164383423605573</v>
+      </c>
+      <c r="G180">
+        <v>0.25387675147930172</v>
+      </c>
+      <c r="H180">
+        <v>0.24059392935896284</v>
+      </c>
+      <c r="J180">
+        <v>0.48627218283396079</v>
+      </c>
+      <c r="K180">
+        <v>0.51241327434104966</v>
+      </c>
+      <c r="L180" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>